<commit_message>
Full update of gold profiles
git-svn-id: http://svn.delph-in.net/erg/trunk@27100 3df82f5b-d43a-0410-af33-fce91db48ec5
</commit_message>
<xml_diff>
--- a/educ/ParserErrorCodes.xlsx
+++ b/educ/ParserErrorCodes.xlsx
@@ -5,10 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet4" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="585">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="601">
   <si>
     <t xml:space="preserve">Situation</t>
   </si>
@@ -118,7 +121,7 @@
     <t xml:space="preserve">v_np-vp_bse_le_rbst, v_vp_seq-bse_le_rbst, j_vp_bse_dlr_rbst, v_vp_ssr-nimp_le_rbst, need_bse_v1_rbst</t>
   </si>
   <si>
-    <t xml:space="preserve">She told her brother borrow her book. She tried read books. She was ready read books. She tends win. We need buy books.</t>
+    <t xml:space="preserve">She told her brother borrow her book. She tried read books. She was ready read books. She tends win. They need buy books.</t>
   </si>
   <si>
     <t xml:space="preserve">The student uses "to" with a verb with which it is not appropriate.</t>
@@ -550,7 +553,7 @@
     <t xml:space="preserve">np-np_crd-im_c_rbst, n-n_crd-im_c_rbst</t>
   </si>
   <si>
-    <t xml:space="preserve">Dogs, cats and mice ran.</t>
+    <t xml:space="preserve">Dogs, cats and mice appeared.</t>
   </si>
   <si>
     <t xml:space="preserve">The student uses the past participle in place of the past form.</t>
@@ -763,7 +766,7 @@
     <t xml:space="preserve">after_pp_rbst</t>
   </si>
   <si>
-    <t xml:space="preserve">After, we bought books.</t>
+    <t xml:space="preserve">We bought books after.</t>
   </si>
   <si>
     <t xml:space="preserve">The student has an NP complement of a verb that requires a sentential complement.</t>
@@ -1132,7 +1135,7 @@
     <t xml:space="preserve">very_asleep_a1_rbst, well_asleep_a1_rbst</t>
   </si>
   <si>
-    <t xml:space="preserve">He is well asleep.</t>
+    <t xml:space="preserve">People well asleep snore.</t>
   </si>
   <si>
     <t xml:space="preserve">The student uses a non-idiomaitc modifier with “awake”.</t>
@@ -1555,12 +1558,6 @@
     <t xml:space="preserve">She will propose that he leaves.</t>
   </si>
   <si>
-    <t xml:space="preserve">if_i_was_you_rbst</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If I was you, I would not go.</t>
-  </si>
-  <si>
     <t xml:space="preserve">The student uses the wrong form of the verb.</t>
   </si>
   <si>
@@ -1720,7 +1717,7 @@
     <t xml:space="preserve">sigh_sign_v1_rbst, fourth_adj_rbst, fourth_day_rbst</t>
   </si>
   <si>
-    <t xml:space="preserve">Students should sigh their names.</t>
+    <t xml:space="preserve">He refused to sigh the form.</t>
   </si>
   <si>
     <t xml:space="preserve">The student omits the object of a preposition.</t>
@@ -1747,7 +1744,7 @@
     <t xml:space="preserve">time_cmpd_n1_rbst</t>
   </si>
   <si>
-    <t xml:space="preserve">This is my second time visit.</t>
+    <t xml:space="preserve">That was my second time win.</t>
   </si>
   <si>
     <t xml:space="preserve">The student adds a spurious “in”.</t>
@@ -1775,6 +1772,60 @@
   </si>
   <si>
     <t xml:space="preserve">Here comes he.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The student uses lower case for the sentence-initial word.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">w_noinitcap_dlr_rbst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the cat slept.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The student omits the matching right comma in apposition.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hdn-np_app-rbc_c_rbst, hdn-np_app-idf-rbc_c_rbst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">His brother, the plumber arrived.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The student may be overusing topicalization.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">flr-hd_nwh_c_rbst, vp_sbrd-pre_c_rbst, as_prd_rbst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As for the new proposal, it should be discussed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The student substitutes a full NP for expletive-it subject.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aj_vp_i-seq_le_rbst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kim is difficult to talk to her.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The student misuses the there-copula construction.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">there_are_adv1_rbst, there_is_adv1_rbst, there_is_cx_adv1_rbst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There are many people admire her.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The student replaces there-copula with `have’.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">be_th_cop_is_has_rbst, be_th_cop_are_have_rbst, be_th_cop_was_had_rbst, be_th_cop_were_had_rbst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There have many solutions for this problem.</t>
   </si>
 </sst>
 </file>
@@ -1789,7 +1840,7 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="2"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
@@ -1811,19 +1862,19 @@
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Noto sans cjk sc regular"/>
-      <family val="2"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -1992,20 +2043,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T201"/>
+  <dimension ref="A1:T207"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A194" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C206" activeCellId="0" sqref="C206"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.1785714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.4489795918367"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.4285714285714"/>
-    <col collapsed="false" hidden="false" max="13" min="4" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="20" min="14" style="0" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="13.9030612244898"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="37.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="30.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="4" style="0" width="8.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="14" style="0" width="8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1018" min="21" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1019" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="53.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6932,15 +6984,15 @@
       <c r="S176" s="2"/>
       <c r="T176" s="2"/>
     </row>
-    <row r="177" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="177" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A177" s="2" t="s">
-        <v>508</v>
+        <v>511</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="D177" s="2"/>
       <c r="E177" s="2"/>
@@ -6960,15 +7012,15 @@
       <c r="S177" s="2"/>
       <c r="T177" s="2"/>
     </row>
-    <row r="178" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="178" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A178" s="2" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="D178" s="2"/>
       <c r="E178" s="2"/>
@@ -6988,15 +7040,15 @@
       <c r="S178" s="2"/>
       <c r="T178" s="2"/>
     </row>
-    <row r="179" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="179" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A179" s="2" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="D179" s="2"/>
       <c r="E179" s="2"/>
@@ -7016,15 +7068,15 @@
       <c r="S179" s="2"/>
       <c r="T179" s="2"/>
     </row>
-    <row r="180" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="180" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A180" s="2" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="D180" s="2"/>
       <c r="E180" s="2"/>
@@ -7046,13 +7098,13 @@
     </row>
     <row r="181" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A181" s="2" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="D181" s="2"/>
       <c r="E181" s="2"/>
@@ -7072,15 +7124,15 @@
       <c r="S181" s="2"/>
       <c r="T181" s="2"/>
     </row>
-    <row r="182" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="182" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A182" s="2" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="D182" s="2"/>
       <c r="E182" s="2"/>
@@ -7102,13 +7154,13 @@
     </row>
     <row r="183" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A183" s="2" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="C183" s="2" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="D183" s="2"/>
       <c r="E183" s="2"/>
@@ -7130,13 +7182,13 @@
     </row>
     <row r="184" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A184" s="2" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="D184" s="2"/>
       <c r="E184" s="2"/>
@@ -7156,15 +7208,15 @@
       <c r="S184" s="2"/>
       <c r="T184" s="2"/>
     </row>
-    <row r="185" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="185" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A185" s="2" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="C185" s="2" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="D185" s="2"/>
       <c r="E185" s="2"/>
@@ -7186,13 +7238,13 @@
     </row>
     <row r="186" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A186" s="2" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="D186" s="2"/>
       <c r="E186" s="2"/>
@@ -7214,13 +7266,13 @@
     </row>
     <row r="187" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A187" s="2" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="D187" s="2"/>
       <c r="E187" s="2"/>
@@ -7242,13 +7294,13 @@
     </row>
     <row r="188" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A188" s="2" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="C188" s="2" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="D188" s="2"/>
       <c r="E188" s="2"/>
@@ -7268,15 +7320,15 @@
       <c r="S188" s="2"/>
       <c r="T188" s="2"/>
     </row>
-    <row r="189" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="189" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A189" s="2" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="C189" s="2" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="D189" s="2"/>
       <c r="E189" s="2"/>
@@ -7298,13 +7350,13 @@
     </row>
     <row r="190" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A190" s="2" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="C190" s="2" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="D190" s="2"/>
       <c r="E190" s="2"/>
@@ -7324,15 +7376,15 @@
       <c r="S190" s="2"/>
       <c r="T190" s="2"/>
     </row>
-    <row r="191" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="191" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A191" s="2" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="C191" s="2" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="D191" s="2"/>
       <c r="E191" s="2"/>
@@ -7352,15 +7404,15 @@
       <c r="S191" s="2"/>
       <c r="T191" s="2"/>
     </row>
-    <row r="192" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="192" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A192" s="2" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="B192" s="2" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="C192" s="2" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="D192" s="2"/>
       <c r="E192" s="2"/>
@@ -7382,13 +7434,13 @@
     </row>
     <row r="193" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A193" s="2" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="C193" s="2" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="D193" s="2"/>
       <c r="E193" s="2"/>
@@ -7408,15 +7460,15 @@
       <c r="S193" s="2"/>
       <c r="T193" s="2"/>
     </row>
-    <row r="194" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="194" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A194" s="2" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="B194" s="2" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="C194" s="2" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="D194" s="2"/>
       <c r="E194" s="2"/>
@@ -7438,13 +7490,13 @@
     </row>
     <row r="195" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A195" s="2" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="B195" s="2" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="C195" s="2" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="D195" s="2"/>
       <c r="E195" s="2"/>
@@ -7466,13 +7518,13 @@
     </row>
     <row r="196" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A196" s="2" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="B196" s="2" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="C196" s="2" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="D196" s="2"/>
       <c r="E196" s="2"/>
@@ -7494,13 +7546,13 @@
     </row>
     <row r="197" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A197" s="2" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="B197" s="2" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="C197" s="2" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="D197" s="2"/>
       <c r="E197" s="2"/>
@@ -7520,15 +7572,15 @@
       <c r="S197" s="2"/>
       <c r="T197" s="2"/>
     </row>
-    <row r="198" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="198" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A198" s="2" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="C198" s="2" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="D198" s="2"/>
       <c r="E198" s="2"/>
@@ -7548,15 +7600,15 @@
       <c r="S198" s="2"/>
       <c r="T198" s="2"/>
     </row>
-    <row r="199" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="199" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A199" s="2" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="C199" s="2" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="D199" s="2"/>
       <c r="E199" s="2"/>
@@ -7578,13 +7630,13 @@
     </row>
     <row r="200" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A200" s="2" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="B200" s="2" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="C200" s="2" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="D200" s="2"/>
       <c r="E200" s="2"/>
@@ -7606,13 +7658,13 @@
     </row>
     <row r="201" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A201" s="2" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="C201" s="2" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="D201" s="2"/>
       <c r="E201" s="2"/>
@@ -7632,10 +7684,4083 @@
       <c r="S201" s="2"/>
       <c r="T201" s="2"/>
     </row>
+    <row r="202" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A202" s="2" t="s">
+        <v>586</v>
+      </c>
+      <c r="B202" s="2" t="s">
+        <v>587</v>
+      </c>
+      <c r="C202" s="2" t="s">
+        <v>588</v>
+      </c>
+      <c r="D202" s="2"/>
+      <c r="E202" s="2"/>
+      <c r="F202" s="2"/>
+      <c r="G202" s="2"/>
+      <c r="H202" s="2"/>
+      <c r="I202" s="2"/>
+      <c r="J202" s="2"/>
+      <c r="K202" s="2"/>
+      <c r="L202" s="2"/>
+      <c r="M202" s="2"/>
+      <c r="N202" s="2"/>
+      <c r="O202" s="2"/>
+      <c r="P202" s="2"/>
+      <c r="Q202" s="2"/>
+      <c r="R202" s="2"/>
+      <c r="S202" s="2"/>
+      <c r="T202" s="2"/>
+    </row>
+    <row r="203" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A203" s="2" t="s">
+        <v>589</v>
+      </c>
+      <c r="B203" s="2" t="s">
+        <v>590</v>
+      </c>
+      <c r="C203" s="2" t="s">
+        <v>591</v>
+      </c>
+      <c r="D203" s="2"/>
+      <c r="E203" s="2"/>
+      <c r="F203" s="2"/>
+      <c r="G203" s="2"/>
+      <c r="H203" s="2"/>
+      <c r="I203" s="2"/>
+      <c r="J203" s="2"/>
+      <c r="K203" s="2"/>
+      <c r="L203" s="2"/>
+      <c r="M203" s="2"/>
+      <c r="N203" s="2"/>
+      <c r="O203" s="2"/>
+      <c r="P203" s="2"/>
+      <c r="Q203" s="2"/>
+      <c r="R203" s="2"/>
+      <c r="S203" s="2"/>
+      <c r="T203" s="2"/>
+    </row>
+    <row r="204" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A204" s="2" t="s">
+        <v>592</v>
+      </c>
+      <c r="B204" s="2" t="s">
+        <v>593</v>
+      </c>
+      <c r="C204" s="2" t="s">
+        <v>594</v>
+      </c>
+      <c r="D204" s="2"/>
+      <c r="E204" s="2"/>
+      <c r="F204" s="2"/>
+      <c r="G204" s="2"/>
+      <c r="H204" s="2"/>
+      <c r="I204" s="2"/>
+      <c r="J204" s="2"/>
+      <c r="K204" s="2"/>
+      <c r="L204" s="2"/>
+      <c r="M204" s="2"/>
+      <c r="N204" s="2"/>
+      <c r="O204" s="2"/>
+      <c r="P204" s="2"/>
+      <c r="Q204" s="2"/>
+      <c r="R204" s="2"/>
+      <c r="S204" s="2"/>
+      <c r="T204" s="2"/>
+    </row>
+    <row r="205" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A205" s="2" t="s">
+        <v>595</v>
+      </c>
+      <c r="B205" s="2" t="s">
+        <v>596</v>
+      </c>
+      <c r="C205" s="2" t="s">
+        <v>597</v>
+      </c>
+      <c r="D205" s="2"/>
+      <c r="E205" s="2"/>
+      <c r="F205" s="2"/>
+      <c r="G205" s="2"/>
+      <c r="H205" s="2"/>
+      <c r="I205" s="2"/>
+      <c r="J205" s="2"/>
+      <c r="K205" s="2"/>
+      <c r="L205" s="2"/>
+      <c r="M205" s="2"/>
+      <c r="N205" s="2"/>
+      <c r="O205" s="2"/>
+      <c r="P205" s="2"/>
+      <c r="Q205" s="2"/>
+      <c r="R205" s="2"/>
+      <c r="S205" s="2"/>
+      <c r="T205" s="2"/>
+    </row>
+    <row r="206" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A206" s="2" t="s">
+        <v>598</v>
+      </c>
+      <c r="B206" s="2" t="s">
+        <v>599</v>
+      </c>
+      <c r="C206" s="2" t="s">
+        <v>600</v>
+      </c>
+      <c r="D206" s="2"/>
+      <c r="E206" s="2"/>
+      <c r="F206" s="2"/>
+      <c r="G206" s="2"/>
+      <c r="H206" s="2"/>
+      <c r="I206" s="2"/>
+      <c r="J206" s="2"/>
+      <c r="K206" s="2"/>
+      <c r="L206" s="2"/>
+      <c r="M206" s="2"/>
+      <c r="N206" s="2"/>
+      <c r="O206" s="2"/>
+      <c r="P206" s="2"/>
+      <c r="Q206" s="2"/>
+      <c r="R206" s="2"/>
+      <c r="S206" s="2"/>
+      <c r="T206" s="2"/>
+    </row>
+    <row r="207" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="208" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="209" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="210" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="211" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="212" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="213" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="214" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="215" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="216" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="217" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="218" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="219" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="220" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="221" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="222" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="223" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="224" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="225" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="226" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="227" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="228" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="229" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="230" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="231" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="232" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="233" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="234" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="235" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="236" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="237" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="238" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="239" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="240" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="241" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="242" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="243" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="244" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="245" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="246" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="247" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="248" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="249" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="250" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="251" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="252" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="253" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="254" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="255" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="256" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="257" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="258" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="259" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="260" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="261" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="262" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="263" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="264" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="265" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="266" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="267" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="268" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="269" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="270" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="271" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="272" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="273" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="274" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="275" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="276" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="277" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="278" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="279" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="280" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="281" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="282" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="283" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="284" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="285" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="286" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="287" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="288" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="289" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="290" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="291" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="292" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="293" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="294" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="295" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="296" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="297" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="298" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="299" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="300" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="301" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="302" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="303" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="304" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="305" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="306" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="307" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="308" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="309" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="310" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="311" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="312" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="313" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="314" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="315" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="316" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="317" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="318" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="319" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="320" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="321" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="322" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="323" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="324" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="325" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="326" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="327" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="328" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="329" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="330" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="331" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="332" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="333" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="334" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="335" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="336" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="337" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="338" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="339" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="340" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="341" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="342" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="343" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="344" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="345" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="346" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="347" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="348" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="349" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="350" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="351" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="352" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="353" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="354" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="355" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="356" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="357" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="358" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="359" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="360" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="361" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="362" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="363" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="364" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="365" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="366" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="367" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="368" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="369" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="370" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="371" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="372" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="373" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="374" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="375" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="376" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="377" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="378" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="379" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="380" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="381" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="382" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="383" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="384" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="385" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="386" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="387" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="388" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="389" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="390" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="391" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="392" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="393" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="394" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="395" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="396" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="397" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="398" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="399" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="400" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="401" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="402" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="403" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="404" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="405" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="406" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="407" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="408" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="409" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="410" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="411" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="412" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="413" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="414" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="415" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="416" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="417" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="418" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="419" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="420" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="421" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="422" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="423" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="424" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="425" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="426" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="427" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="428" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="429" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="430" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="431" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="432" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="433" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="434" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="435" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="436" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="437" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="438" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="439" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="440" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="441" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="442" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="443" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="444" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="445" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="446" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="447" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="448" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="449" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="450" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="451" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="452" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="453" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="454" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="455" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="456" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="457" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="458" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="459" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="460" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="461" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="462" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="463" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="464" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="465" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="466" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="467" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="468" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="469" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="470" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="471" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="472" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="473" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="474" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="475" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="476" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="477" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="478" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="479" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="480" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="481" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="482" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="483" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="484" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="485" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="486" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="487" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="488" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="489" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="490" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="491" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="492" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="493" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="494" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="495" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="496" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="497" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="498" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="499" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="500" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="501" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="502" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="503" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="504" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="505" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="506" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="507" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="508" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="509" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="510" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="511" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="512" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="513" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="514" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="515" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="516" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="517" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="518" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="519" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="520" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="521" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="522" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="523" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="524" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="525" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="526" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="527" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="528" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="529" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="530" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="531" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="532" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="533" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="534" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="535" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="536" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="537" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="538" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="539" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="540" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="541" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="542" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="543" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="544" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="545" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="546" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="547" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="548" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="549" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="550" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="551" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="552" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="553" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="554" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="555" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="556" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="557" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="558" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="559" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="560" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="561" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="562" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="563" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="564" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="565" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="566" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="567" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="568" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="569" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="570" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="571" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="572" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="573" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="574" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="575" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="576" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="577" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="578" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="579" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="580" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="581" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="582" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="583" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="584" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="585" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="586" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="587" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="588" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="589" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="590" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="591" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="592" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="593" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="594" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="595" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="596" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="597" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="598" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="599" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="600" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="601" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="602" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="603" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="604" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="605" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="606" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="607" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="608" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="609" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="610" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="611" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="612" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="613" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="614" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="615" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="616" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="617" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="618" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="619" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="620" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="621" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="622" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="623" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="624" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="625" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="626" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="627" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="628" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="629" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="630" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="631" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="632" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="633" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="634" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="635" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="636" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="637" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="638" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="639" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="640" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="641" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="642" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="643" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="644" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="645" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="646" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="647" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="648" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="649" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="650" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="651" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="652" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="653" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="654" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="655" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="656" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="657" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="658" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="659" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="660" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="661" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="662" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="663" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="664" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="665" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="666" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="667" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="668" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="669" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="670" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="671" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="672" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="673" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="674" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="675" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="676" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="677" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="678" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="679" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="680" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="681" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="682" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="683" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="684" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="685" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="686" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="687" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="688" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="689" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="690" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="691" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="692" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="693" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="694" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="695" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="696" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="697" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="698" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="699" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="700" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="701" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="702" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="703" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="704" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="705" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="706" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="707" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="708" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="709" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="710" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="711" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="712" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="713" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="714" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="715" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="716" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="717" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="718" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="719" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="720" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="721" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="722" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="723" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="724" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="725" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="726" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="727" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="728" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="729" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="730" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="731" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="732" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="733" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="734" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="735" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="736" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="737" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="738" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="739" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="740" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="741" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="742" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="743" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="744" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="745" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="746" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="747" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="748" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="749" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="750" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="751" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="752" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="753" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="754" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="755" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="756" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="757" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="758" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="759" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="760" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="761" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="762" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="763" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="764" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="765" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="766" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="767" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="768" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="769" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="770" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="771" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="772" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="773" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="774" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="775" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="776" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="777" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="778" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="779" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="780" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="781" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="782" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="783" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="784" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="785" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="786" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="787" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="788" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="789" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="790" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="791" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="792" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="793" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="794" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="795" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="796" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="797" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="798" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="799" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="800" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="801" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="802" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="803" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="804" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="805" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="806" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="807" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="808" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="809" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="810" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="811" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="812" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="813" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="814" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="815" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="816" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="817" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="818" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="819" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="820" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="821" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="822" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="823" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="824" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="825" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="826" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="827" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="828" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="829" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="830" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="831" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="832" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="833" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="834" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="835" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="836" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="837" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="838" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="839" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="840" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="841" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="842" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="843" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="844" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="845" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="846" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="847" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="848" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="849" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="850" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="851" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="852" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="853" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="854" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="855" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="856" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="857" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="858" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="859" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="860" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="861" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="862" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="863" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="864" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="865" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="866" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="867" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="868" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="869" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="870" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="871" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="872" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="873" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="874" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="875" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="876" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="877" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="878" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="879" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="880" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="881" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="882" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="883" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="884" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="885" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="886" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="887" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="888" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="889" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="890" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="891" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="892" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="893" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="894" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="895" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="896" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="897" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="898" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="899" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="900" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="901" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="902" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="903" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="904" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="905" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="906" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="907" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="908" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="909" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="910" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="911" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="912" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="913" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="914" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="915" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="916" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="917" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="918" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="919" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="920" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="921" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="922" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="923" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="924" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="925" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="926" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="927" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="928" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="929" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="930" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="931" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="932" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="933" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="934" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="935" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="936" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="937" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="938" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="939" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="940" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="941" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="942" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="943" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="944" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="945" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="946" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="947" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="948" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="949" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="950" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="951" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="952" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="953" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="954" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="955" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="956" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="957" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="958" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="959" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="960" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="961" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="962" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="963" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="964" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="965" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="966" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="967" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="968" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="969" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="970" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="971" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="972" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="973" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="974" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="975" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="976" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="977" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="978" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="979" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="980" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="981" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="982" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="983" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="984" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="985" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="986" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="987" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="988" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="989" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="990" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="991" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="992" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="993" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="994" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="995" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="996" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="997" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="998" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="999" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="1" style="0" width="8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="0" width="14.43"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="2" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="3" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="4" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="5" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="6" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="7" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="22" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="24" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="26" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="27" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="28" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="30" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="31" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="32" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="33" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="34" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="35" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="36" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="37" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="38" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="39" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="40" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="41" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="42" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="43" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="44" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="45" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="46" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="47" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="48" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="49" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="50" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="51" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="52" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="53" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="54" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="55" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="56" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="57" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="58" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="59" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="60" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="61" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="62" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="63" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="64" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="65" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="66" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="67" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="68" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="69" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="70" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="71" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="72" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="73" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="74" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="75" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="76" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="77" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="78" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="79" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="80" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="81" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="82" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="83" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="84" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="85" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="86" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="87" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="88" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="89" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="90" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="91" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="92" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="93" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="94" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="95" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="96" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="97" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="98" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="99" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="100" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="101" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="102" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="103" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="104" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="105" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="106" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="107" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="108" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="109" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="110" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="111" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="112" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="113" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="114" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="115" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="116" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="117" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="118" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="119" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="120" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="121" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="122" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="123" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="124" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="125" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="126" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="127" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="128" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="129" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="130" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="131" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="132" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="133" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="134" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="135" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="136" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="137" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="138" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="139" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="140" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="141" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="142" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="143" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="144" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="145" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="146" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="147" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="148" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="149" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="150" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="151" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="152" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="153" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="154" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="155" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="156" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="157" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="158" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="159" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="160" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="161" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="162" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="163" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="164" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="165" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="166" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="167" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="168" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="169" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="170" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="171" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="172" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="173" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="174" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="175" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="176" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="177" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="178" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="179" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="180" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="181" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="182" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="183" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="184" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="185" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="186" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="187" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="188" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="189" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="190" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="191" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="192" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="193" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="194" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="195" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="196" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="197" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="198" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="199" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="200" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="201" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="202" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="203" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="204" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="205" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="206" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="207" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="208" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="209" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="210" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="211" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="212" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="213" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="214" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="215" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="216" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="217" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="218" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="219" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="220" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="221" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="222" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="223" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="224" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="225" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="226" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="227" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="228" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="229" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="230" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="231" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="232" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="233" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="234" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="235" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="236" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="237" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="238" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="239" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="240" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="241" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="242" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="243" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="244" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="245" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="246" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="247" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="248" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="249" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="250" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="251" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="252" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="253" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="254" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="255" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="256" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="257" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="258" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="259" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="260" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="261" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="262" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="263" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="264" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="265" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="266" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="267" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="268" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="269" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="270" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="271" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="272" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="273" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="274" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="275" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="276" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="277" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="278" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="279" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="280" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="281" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="282" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="283" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="284" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="285" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="286" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="287" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="288" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="289" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="290" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="291" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="292" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="293" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="294" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="295" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="296" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="297" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="298" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="299" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="300" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="301" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="302" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="303" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="304" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="305" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="306" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="307" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="308" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="309" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="310" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="311" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="312" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="313" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="314" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="315" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="316" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="317" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="318" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="319" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="320" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="321" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="322" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="323" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="324" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="325" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="326" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="327" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="328" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="329" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="330" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="331" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="332" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="333" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="334" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="335" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="336" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="337" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="338" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="339" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="340" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="341" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="342" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="343" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="344" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="345" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="346" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="347" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="348" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="349" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="350" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="351" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="352" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="353" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="354" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="355" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="356" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="357" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="358" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="359" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="360" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="361" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="362" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="363" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="364" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="365" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="366" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="367" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="368" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="369" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="370" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="371" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="372" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="373" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="374" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="375" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="376" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="377" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="378" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="379" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="380" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="381" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="382" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="383" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="384" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="385" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="386" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="387" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="388" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="389" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="390" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="391" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="392" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="393" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="394" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="395" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="396" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="397" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="398" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="399" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="400" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="401" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="402" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="403" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="404" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="405" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="406" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="407" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="408" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="409" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="410" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="411" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="412" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="413" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="414" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="415" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="416" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="417" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="418" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="419" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="420" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="421" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="422" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="423" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="424" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="425" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="426" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="427" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="428" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="429" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="430" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="431" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="432" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="433" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="434" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="435" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="436" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="437" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="438" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="439" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="440" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="441" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="442" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="443" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="444" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="445" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="446" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="447" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="448" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="449" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="450" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="451" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="452" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="453" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="454" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="455" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="456" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="457" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="458" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="459" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="460" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="461" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="462" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="463" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="464" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="465" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="466" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="467" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="468" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="469" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="470" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="471" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="472" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="473" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="474" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="475" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="476" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="477" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="478" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="479" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="480" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="481" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="482" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="483" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="484" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="485" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="486" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="487" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="488" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="489" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="490" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="491" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="492" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="493" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="494" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="495" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="496" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="497" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="498" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="499" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="500" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="501" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="502" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="503" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="504" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="505" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="506" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="507" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="508" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="509" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="510" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="511" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="512" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="513" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="514" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="515" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="516" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="517" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="518" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="519" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="520" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="521" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="522" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="523" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="524" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="525" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="526" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="527" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="528" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="529" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="530" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="531" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="532" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="533" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="534" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="535" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="536" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="537" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="538" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="539" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="540" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="541" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="542" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="543" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="544" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="545" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="546" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="547" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="548" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="549" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="550" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="551" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="552" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="553" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="554" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="555" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="556" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="557" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="558" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="559" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="560" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="561" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="562" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="563" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="564" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="565" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="566" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="567" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="568" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="569" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="570" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="571" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="572" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="573" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="574" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="575" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="576" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="577" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="578" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="579" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="580" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="581" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="582" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="583" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="584" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="585" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="586" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="587" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="588" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="589" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="590" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="591" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="592" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="593" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="594" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="595" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="596" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="597" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="598" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="599" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="600" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="601" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="602" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="603" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="604" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="605" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="606" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="607" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="608" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="609" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="610" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="611" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="612" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="613" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="614" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="615" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="616" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="617" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="618" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="619" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="620" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="621" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="622" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="623" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="624" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="625" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="626" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="627" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="628" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="629" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="630" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="631" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="632" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="633" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="634" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="635" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="636" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="637" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="638" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="639" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="640" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="641" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="642" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="643" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="644" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="645" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="646" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="647" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="648" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="649" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="650" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="651" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="652" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="653" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="654" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="655" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="656" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="657" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="658" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="659" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="660" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="661" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="662" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="663" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="664" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="665" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="666" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="667" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="668" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="669" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="670" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="671" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="672" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="673" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="674" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="675" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="676" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="677" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="678" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="679" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="680" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="681" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="682" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="683" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="684" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="685" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="686" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="687" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="688" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="689" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="690" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="691" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="692" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="693" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="694" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="695" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="696" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="697" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="698" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="699" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="700" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="701" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="702" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="703" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="704" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="705" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="706" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="707" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="708" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="709" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="710" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="711" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="712" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="713" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="714" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="715" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="716" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="717" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="718" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="719" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="720" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="721" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="722" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="723" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="724" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="725" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="726" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="727" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="728" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="729" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="730" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="731" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="732" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="733" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="734" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="735" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="736" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="737" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="738" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="739" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="740" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="741" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="742" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="743" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="744" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="745" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="746" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="747" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="748" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="749" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="750" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="751" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="752" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="753" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="754" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="755" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="756" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="757" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="758" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="759" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="760" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="761" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="762" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="763" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="764" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="765" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="766" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="767" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="768" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="769" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="770" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="771" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="772" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="773" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="774" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="775" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="776" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="777" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="778" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="779" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="780" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="781" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="782" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="783" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="784" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="785" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="786" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="787" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="788" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="789" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="790" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="791" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="792" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="793" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="794" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="795" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="796" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="797" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="798" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="799" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="800" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="801" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="802" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="803" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="804" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="805" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="806" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="807" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="808" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="809" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="810" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="811" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="812" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="813" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="814" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="815" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="816" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="817" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="818" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="819" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="820" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="821" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="822" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="823" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="824" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="825" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="826" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="827" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="828" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="829" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="830" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="831" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="832" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="833" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="834" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="835" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="836" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="837" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="838" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="839" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="840" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="841" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="842" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="843" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="844" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="845" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="846" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="847" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="848" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="849" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="850" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="851" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="852" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="853" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="854" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="855" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="856" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="857" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="858" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="859" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="860" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="861" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="862" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="863" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="864" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="865" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="866" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="867" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="868" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="869" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="870" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="871" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="872" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="873" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="874" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="875" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="876" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="877" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="878" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="879" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="880" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="881" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="882" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="883" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="884" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="885" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="886" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="887" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="888" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="889" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="890" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="891" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="892" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="893" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="894" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="895" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="896" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="897" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="898" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="899" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="900" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="901" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="902" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="903" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="904" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="905" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="906" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="907" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="908" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="909" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="910" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="911" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="912" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="913" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="914" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="915" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="916" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="917" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="918" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="919" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="920" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="921" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="922" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="923" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="924" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="925" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="926" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="927" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="928" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="929" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="930" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="931" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="932" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="933" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="934" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="935" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="936" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="937" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="938" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="939" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="940" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="941" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="942" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="943" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="944" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="945" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="946" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="947" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="948" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="949" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="950" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="951" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="952" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="953" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="954" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="955" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="956" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="957" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="958" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="959" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="960" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="961" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="962" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="963" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="964" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="965" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="966" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="967" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="968" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="969" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="970" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="971" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="972" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="973" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="974" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="975" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="976" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="977" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="978" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="979" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="980" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="981" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="982" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="983" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="984" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="985" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="986" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="987" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="988" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="989" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="990" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="991" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="992" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="993" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="994" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="995" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="996" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="997" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="998" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="999" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1000" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:Z2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="1" style="0" width="8.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="11" style="0" width="8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="0" width="14.43"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
+    </row>
+    <row r="2" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="3" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="4" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="5" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="6" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="7" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="22" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="24" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="26" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="27" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="28" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="30" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="31" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="32" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="33" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="34" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="35" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="36" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="37" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="38" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="39" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="40" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="41" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="42" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="43" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="44" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="45" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="46" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="47" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="48" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="49" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="50" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="51" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="52" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="53" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="54" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="55" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="56" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="57" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="58" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="59" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="60" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="61" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="62" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="63" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="64" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="65" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="66" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="67" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="68" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="69" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="70" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="71" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="72" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="73" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="74" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="75" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="76" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="77" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="78" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="79" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="80" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="81" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="82" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="83" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="84" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="85" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="86" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="87" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="88" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="89" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="90" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="91" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="92" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="93" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="94" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="95" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="96" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="97" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="98" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="99" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="100" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="101" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="102" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="103" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="104" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="105" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="106" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="107" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="108" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="109" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="110" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="111" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="112" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="113" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="114" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="115" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="116" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="117" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="118" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="119" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="120" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="121" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="122" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="123" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="124" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="125" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="126" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="127" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="128" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="129" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="130" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="131" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="132" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="133" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="134" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="135" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="136" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="137" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="138" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="139" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="140" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="141" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="142" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="143" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="144" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="145" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="146" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="147" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="148" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="149" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="150" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="151" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="152" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="153" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="154" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="155" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="156" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="157" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="158" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="159" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="160" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="161" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="162" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="163" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="164" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="165" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="166" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="167" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="168" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="169" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="170" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="171" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="172" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="173" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="174" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="175" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="176" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="177" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="178" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="179" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="180" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="181" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="182" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="183" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="184" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="185" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="186" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="187" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="188" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="189" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="190" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="191" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="192" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="193" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="194" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="195" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="196" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="197" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="198" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="199" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="200" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="201" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="202" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="203" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="204" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="205" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="206" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="207" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="208" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="209" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="210" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="211" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="212" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="213" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="214" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="215" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="216" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="217" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="218" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="219" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="220" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="221" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="222" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="223" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="224" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="225" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="226" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="227" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="228" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="229" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="230" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="231" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="232" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="233" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="234" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="235" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="236" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="237" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="238" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="239" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="240" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="241" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="242" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="243" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="244" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="245" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="246" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="247" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="248" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="249" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="250" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="251" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="252" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="253" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="254" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="255" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="256" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="257" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="258" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="259" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="260" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="261" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="262" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="263" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="264" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="265" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="266" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="267" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="268" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="269" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="270" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="271" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="272" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="273" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="274" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="275" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="276" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="277" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="278" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="279" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="280" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="281" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="282" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="283" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="284" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="285" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="286" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="287" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="288" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="289" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="290" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="291" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="292" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="293" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="294" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="295" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="296" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="297" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="298" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="299" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="300" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="301" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="302" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="303" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="304" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="305" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="306" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="307" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="308" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="309" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="310" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="311" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="312" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="313" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="314" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="315" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="316" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="317" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="318" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="319" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="320" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="321" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="322" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="323" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="324" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="325" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="326" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="327" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="328" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="329" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="330" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="331" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="332" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="333" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="334" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="335" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="336" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="337" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="338" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="339" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="340" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="341" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="342" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="343" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="344" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="345" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="346" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="347" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="348" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="349" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="350" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="351" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="352" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="353" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="354" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="355" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="356" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="357" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="358" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="359" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="360" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="361" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="362" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="363" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="364" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="365" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="366" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="367" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="368" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="369" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="370" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="371" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="372" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="373" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="374" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="375" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="376" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="377" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="378" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="379" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="380" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="381" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="382" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="383" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="384" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="385" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="386" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="387" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="388" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="389" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="390" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="391" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="392" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="393" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="394" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="395" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="396" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="397" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="398" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="399" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="400" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="401" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="402" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="403" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="404" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="405" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="406" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="407" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="408" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="409" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="410" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="411" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="412" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="413" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="414" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="415" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="416" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="417" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="418" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="419" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="420" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="421" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="422" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="423" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="424" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="425" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="426" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="427" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="428" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="429" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="430" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="431" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="432" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="433" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="434" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="435" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="436" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="437" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="438" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="439" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="440" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="441" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="442" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="443" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="444" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="445" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="446" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="447" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="448" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="449" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="450" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="451" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="452" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="453" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="454" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="455" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="456" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="457" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="458" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="459" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="460" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="461" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="462" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="463" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="464" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="465" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="466" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="467" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="468" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="469" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="470" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="471" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="472" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="473" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="474" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="475" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="476" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="477" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="478" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="479" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="480" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="481" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="482" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="483" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="484" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="485" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="486" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="487" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="488" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="489" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="490" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="491" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="492" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="493" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="494" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="495" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="496" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="497" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="498" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="499" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="500" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="501" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="502" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="503" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="504" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="505" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="506" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="507" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="508" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="509" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="510" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="511" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="512" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="513" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="514" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="515" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="516" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="517" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="518" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="519" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="520" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="521" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="522" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="523" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="524" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="525" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="526" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="527" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="528" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="529" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="530" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="531" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="532" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="533" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="534" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="535" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="536" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="537" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="538" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="539" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="540" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="541" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="542" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="543" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="544" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="545" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="546" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="547" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="548" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="549" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="550" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="551" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="552" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="553" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="554" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="555" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="556" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="557" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="558" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="559" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="560" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="561" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="562" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="563" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="564" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="565" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="566" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="567" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="568" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="569" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="570" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="571" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="572" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="573" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="574" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="575" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="576" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="577" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="578" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="579" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="580" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="581" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="582" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="583" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="584" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="585" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="586" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="587" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="588" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="589" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="590" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="591" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="592" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="593" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="594" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="595" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="596" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="597" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="598" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="599" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="600" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="601" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="602" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="603" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="604" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="605" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="606" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="607" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="608" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="609" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="610" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="611" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="612" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="613" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="614" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="615" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="616" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="617" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="618" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="619" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="620" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="621" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="622" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="623" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="624" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="625" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="626" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="627" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="628" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="629" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="630" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="631" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="632" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="633" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="634" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="635" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="636" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="637" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="638" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="639" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="640" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="641" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="642" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="643" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="644" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="645" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="646" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="647" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="648" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="649" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="650" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="651" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="652" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="653" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="654" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="655" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="656" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="657" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="658" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="659" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="660" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="661" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="662" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="663" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="664" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="665" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="666" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="667" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="668" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="669" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="670" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="671" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="672" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="673" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="674" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="675" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="676" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="677" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="678" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="679" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="680" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="681" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="682" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="683" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="684" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="685" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="686" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="687" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="688" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="689" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="690" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="691" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="692" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="693" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="694" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="695" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="696" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="697" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="698" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="699" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="700" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="701" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="702" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="703" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="704" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="705" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="706" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="707" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="708" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="709" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="710" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="711" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="712" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="713" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="714" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="715" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="716" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="717" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="718" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="719" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="720" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="721" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="722" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="723" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="724" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="725" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="726" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="727" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="728" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="729" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="730" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="731" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="732" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="733" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="734" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="735" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="736" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="737" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="738" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="739" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="740" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="741" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="742" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="743" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="744" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="745" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="746" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="747" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="748" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="749" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="750" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="751" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="752" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="753" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="754" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="755" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="756" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="757" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="758" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="759" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="760" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="761" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="762" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="763" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="764" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="765" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="766" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="767" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="768" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="769" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="770" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="771" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="772" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="773" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="774" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="775" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="776" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="777" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="778" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="779" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="780" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="781" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="782" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="783" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="784" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="785" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="786" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="787" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="788" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="789" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="790" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="791" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="792" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="793" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="794" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="795" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="796" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="797" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="798" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="799" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="800" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="801" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="802" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="803" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="804" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="805" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="806" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="807" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="808" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="809" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="810" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="811" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="812" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="813" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="814" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="815" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="816" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="817" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="818" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="819" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="820" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="821" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="822" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="823" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="824" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="825" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="826" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="827" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="828" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="829" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="830" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="831" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="832" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="833" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="834" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="835" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="836" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="837" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="838" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="839" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="840" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="841" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="842" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="843" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="844" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="845" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="846" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="847" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="848" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="849" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="850" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="851" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="852" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="853" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="854" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="855" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="856" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="857" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="858" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="859" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="860" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="861" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="862" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="863" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="864" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="865" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="866" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="867" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="868" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="869" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="870" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="871" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="872" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="873" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="874" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="875" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="876" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="877" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="878" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="879" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="880" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="881" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="882" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="883" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="884" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="885" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="886" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="887" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="888" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="889" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="890" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="891" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="892" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="893" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="894" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="895" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="896" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="897" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="898" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="899" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="900" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="901" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="902" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="903" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="904" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="905" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="906" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="907" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="908" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="909" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="910" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="911" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="912" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="913" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="914" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="915" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="916" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="917" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="918" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="919" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="920" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="921" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="922" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="923" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="924" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="925" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="926" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="927" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="928" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="929" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="930" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="931" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="932" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="933" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="934" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="935" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="936" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="937" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="938" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="939" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="940" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="941" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="942" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="943" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="944" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="945" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="946" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="947" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="948" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="949" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="950" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="951" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="952" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="953" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="954" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="955" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="956" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="957" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="958" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="959" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="960" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="961" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="962" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="963" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="964" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="965" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="966" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="967" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="968" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="969" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="970" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="971" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="972" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="973" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="974" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="975" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="976" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="977" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="978" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="979" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="980" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="981" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="982" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="983" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="984" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="985" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="986" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="987" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="988" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="989" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="990" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="991" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="992" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="993" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="994" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="995" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="996" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="997" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="998" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="999" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1000" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:Z2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="1" style="0" width="8.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="11" style="0" width="8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="0" width="14.43"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
+    </row>
+    <row r="2" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="3" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="4" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="5" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="6" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="7" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="22" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="24" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="26" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="27" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="28" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="30" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="31" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="32" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="33" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="34" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="35" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="36" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="37" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="38" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="39" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="40" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="41" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="42" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="43" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="44" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="45" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="46" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="47" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="48" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="49" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="50" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="51" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="52" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="53" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="54" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="55" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="56" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="57" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="58" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="59" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="60" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="61" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="62" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="63" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="64" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="65" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="66" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="67" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="68" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="69" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="70" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="71" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="72" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="73" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="74" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="75" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="76" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="77" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="78" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="79" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="80" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="81" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="82" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="83" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="84" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="85" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="86" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="87" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="88" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="89" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="90" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="91" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="92" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="93" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="94" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="95" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="96" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="97" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="98" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="99" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="100" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="101" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="102" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="103" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="104" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="105" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="106" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="107" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="108" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="109" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="110" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="111" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="112" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="113" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="114" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="115" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="116" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="117" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="118" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="119" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="120" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="121" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="122" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="123" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="124" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="125" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="126" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="127" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="128" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="129" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="130" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="131" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="132" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="133" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="134" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="135" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="136" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="137" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="138" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="139" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="140" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="141" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="142" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="143" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="144" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="145" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="146" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="147" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="148" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="149" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="150" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="151" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="152" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="153" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="154" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="155" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="156" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="157" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="158" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="159" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="160" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="161" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="162" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="163" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="164" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="165" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="166" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="167" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="168" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="169" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="170" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="171" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="172" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="173" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="174" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="175" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="176" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="177" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="178" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="179" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="180" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="181" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="182" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="183" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="184" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="185" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="186" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="187" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="188" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="189" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="190" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="191" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="192" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="193" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="194" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="195" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="196" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="197" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="198" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="199" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="200" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="201" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="202" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="203" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="204" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="205" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="206" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="207" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="208" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="209" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="210" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="211" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="212" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="213" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="214" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="215" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="216" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="217" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="218" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="219" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="220" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="221" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="222" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="223" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="224" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="225" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="226" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="227" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="228" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="229" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="230" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="231" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="232" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="233" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="234" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="235" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="236" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="237" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="238" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="239" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="240" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="241" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="242" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="243" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="244" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="245" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="246" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="247" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="248" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="249" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="250" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="251" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="252" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="253" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="254" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="255" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="256" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="257" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="258" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="259" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="260" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="261" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="262" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="263" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="264" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="265" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="266" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="267" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="268" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="269" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="270" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="271" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="272" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="273" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="274" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="275" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="276" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="277" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="278" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="279" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="280" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="281" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="282" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="283" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="284" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="285" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="286" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="287" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="288" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="289" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="290" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="291" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="292" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="293" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="294" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="295" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="296" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="297" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="298" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="299" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="300" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="301" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="302" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="303" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="304" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="305" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="306" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="307" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="308" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="309" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="310" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="311" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="312" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="313" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="314" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="315" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="316" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="317" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="318" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="319" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="320" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="321" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="322" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="323" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="324" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="325" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="326" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="327" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="328" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="329" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="330" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="331" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="332" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="333" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="334" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="335" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="336" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="337" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="338" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="339" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="340" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="341" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="342" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="343" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="344" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="345" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="346" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="347" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="348" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="349" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="350" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="351" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="352" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="353" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="354" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="355" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="356" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="357" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="358" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="359" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="360" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="361" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="362" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="363" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="364" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="365" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="366" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="367" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="368" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="369" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="370" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="371" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="372" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="373" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="374" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="375" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="376" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="377" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="378" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="379" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="380" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="381" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="382" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="383" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="384" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="385" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="386" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="387" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="388" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="389" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="390" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="391" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="392" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="393" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="394" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="395" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="396" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="397" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="398" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="399" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="400" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="401" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="402" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="403" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="404" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="405" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="406" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="407" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="408" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="409" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="410" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="411" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="412" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="413" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="414" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="415" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="416" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="417" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="418" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="419" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="420" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="421" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="422" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="423" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="424" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="425" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="426" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="427" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="428" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="429" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="430" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="431" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="432" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="433" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="434" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="435" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="436" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="437" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="438" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="439" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="440" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="441" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="442" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="443" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="444" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="445" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="446" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="447" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="448" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="449" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="450" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="451" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="452" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="453" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="454" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="455" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="456" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="457" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="458" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="459" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="460" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="461" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="462" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="463" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="464" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="465" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="466" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="467" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="468" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="469" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="470" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="471" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="472" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="473" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="474" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="475" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="476" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="477" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="478" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="479" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="480" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="481" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="482" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="483" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="484" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="485" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="486" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="487" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="488" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="489" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="490" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="491" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="492" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="493" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="494" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="495" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="496" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="497" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="498" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="499" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="500" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="501" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="502" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="503" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="504" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="505" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="506" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="507" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="508" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="509" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="510" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="511" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="512" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="513" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="514" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="515" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="516" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="517" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="518" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="519" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="520" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="521" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="522" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="523" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="524" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="525" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="526" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="527" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="528" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="529" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="530" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="531" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="532" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="533" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="534" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="535" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="536" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="537" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="538" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="539" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="540" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="541" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="542" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="543" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="544" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="545" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="546" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="547" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="548" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="549" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="550" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="551" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="552" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="553" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="554" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="555" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="556" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="557" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="558" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="559" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="560" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="561" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="562" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="563" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="564" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="565" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="566" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="567" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="568" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="569" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="570" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="571" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="572" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="573" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="574" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="575" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="576" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="577" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="578" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="579" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="580" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="581" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="582" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="583" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="584" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="585" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="586" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="587" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="588" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="589" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="590" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="591" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="592" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="593" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="594" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="595" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="596" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="597" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="598" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="599" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="600" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="601" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="602" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="603" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="604" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="605" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="606" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="607" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="608" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="609" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="610" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="611" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="612" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="613" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="614" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="615" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="616" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="617" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="618" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="619" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="620" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="621" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="622" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="623" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="624" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="625" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="626" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="627" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="628" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="629" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="630" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="631" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="632" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="633" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="634" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="635" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="636" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="637" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="638" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="639" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="640" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="641" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="642" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="643" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="644" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="645" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="646" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="647" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="648" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="649" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="650" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="651" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="652" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="653" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="654" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="655" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="656" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="657" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="658" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="659" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="660" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="661" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="662" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="663" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="664" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="665" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="666" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="667" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="668" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="669" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="670" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="671" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="672" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="673" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="674" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="675" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="676" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="677" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="678" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="679" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="680" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="681" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="682" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="683" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="684" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="685" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="686" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="687" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="688" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="689" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="690" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="691" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="692" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="693" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="694" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="695" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="696" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="697" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="698" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="699" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="700" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="701" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="702" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="703" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="704" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="705" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="706" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="707" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="708" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="709" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="710" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="711" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="712" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="713" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="714" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="715" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="716" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="717" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="718" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="719" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="720" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="721" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="722" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="723" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="724" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="725" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="726" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="727" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="728" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="729" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="730" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="731" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="732" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="733" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="734" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="735" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="736" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="737" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="738" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="739" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="740" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="741" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="742" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="743" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="744" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="745" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="746" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="747" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="748" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="749" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="750" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="751" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="752" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="753" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="754" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="755" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="756" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="757" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="758" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="759" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="760" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="761" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="762" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="763" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="764" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="765" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="766" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="767" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="768" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="769" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="770" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="771" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="772" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="773" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="774" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="775" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="776" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="777" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="778" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="779" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="780" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="781" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="782" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="783" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="784" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="785" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="786" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="787" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="788" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="789" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="790" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="791" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="792" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="793" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="794" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="795" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="796" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="797" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="798" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="799" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="800" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="801" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="802" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="803" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="804" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="805" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="806" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="807" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="808" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="809" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="810" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="811" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="812" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="813" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="814" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="815" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="816" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="817" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="818" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="819" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="820" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="821" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="822" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="823" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="824" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="825" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="826" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="827" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="828" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="829" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="830" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="831" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="832" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="833" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="834" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="835" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="836" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="837" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="838" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="839" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="840" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="841" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="842" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="843" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="844" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="845" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="846" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="847" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="848" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="849" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="850" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="851" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="852" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="853" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="854" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="855" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="856" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="857" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="858" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="859" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="860" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="861" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="862" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="863" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="864" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="865" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="866" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="867" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="868" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="869" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="870" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="871" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="872" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="873" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="874" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="875" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="876" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="877" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="878" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="879" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="880" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="881" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="882" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="883" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="884" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="885" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="886" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="887" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="888" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="889" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="890" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="891" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="892" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="893" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="894" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="895" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="896" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="897" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="898" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="899" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="900" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="901" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="902" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="903" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="904" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="905" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="906" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="907" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="908" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="909" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="910" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="911" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="912" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="913" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="914" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="915" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="916" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="917" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="918" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="919" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="920" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="921" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="922" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="923" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="924" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="925" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="926" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="927" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="928" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="929" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="930" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="931" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="932" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="933" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="934" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="935" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="936" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="937" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="938" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="939" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="940" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="941" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="942" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="943" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="944" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="945" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="946" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="947" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="948" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="949" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="950" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="951" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="952" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="953" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="954" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="955" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="956" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="957" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="958" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="959" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="960" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="961" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="962" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="963" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="964" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="965" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="966" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="967" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="968" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="969" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="970" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="971" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="972" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="973" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="974" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="975" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="976" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="977" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="978" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="979" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="980" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="981" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="982" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="983" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="984" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="985" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="986" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="987" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="988" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="989" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="990" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="991" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="992" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="993" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="994" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="995" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="996" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="997" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="998" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="999" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1000" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
Interim update with better support for openproof and educ, and with more gold profiles for wsj.
git-svn-id: http://svn.delph-in.net/erg/trunk@28199 3df82f5b-d43a-0410-af33-fce91db48ec5
</commit_message>
<xml_diff>
--- a/educ/ParserErrorCodes.xlsx
+++ b/educ/ParserErrorCodes.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="601">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="746">
   <si>
     <t xml:space="preserve">Situation</t>
   </si>
@@ -64,16 +64,16 @@
     <t xml:space="preserve">The student's sentence uses awkward phrasing.</t>
   </si>
   <si>
-    <t xml:space="preserve">adjh_i_inv_rbst, vmod_i_rbst, av_-_i-vp-po_le_rbst,  np_fillhead_non_wh_rbst, pp_fillhead_non_wh_rbst, be_inv_is_rbst, be_inv_are_rbst, be_inv_was_rbst, be_inv_were_rbst, be_inv_be_rbst, because_rbst</t>
-  </si>
-  <si>
-    <t xml:space="preserve">They saw in the lake a duck.</t>
+    <t xml:space="preserve">adjh_i_inv_rbst, vmod_i_rbst, av_-_i-vp-po_le_rbst,  np_fillhead_non_wh_rbst, pp_fillhead_non_wh_rbst, be_inv_is_rbst, be_inv_are_rbst, be_inv_was_rbst, be_inv_were_rbst, be_inv_be_rbst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">They saw in the lake some ducks.</t>
   </si>
   <si>
     <t xml:space="preserve">The student's sentence would be correct, but it is missing an article or a possessive noun or pronoun.</t>
   </si>
   <si>
-    <t xml:space="preserve">hdn_bnp_c_rbst, morning_nospr_n1_rbst, afternoon_nospr_n1_rbst, evening_nospr_n1_rbst</t>
+    <t xml:space="preserve">hdn_bnp_c_rbst, morning_nospr_n1_rbst, afternoon_nospr_n1_rbst, evening_nospr_n1_rbst, n_-_m-nomod_le_rbst</t>
   </si>
   <si>
     <t xml:space="preserve">He went to house.</t>
@@ -91,7 +91,7 @@
     <t xml:space="preserve">The student uses "a" before a vowel sound.</t>
   </si>
   <si>
-    <t xml:space="preserve">a_det_rbst, a_one_adj_rbst</t>
+    <t xml:space="preserve">a_det_rbst, a_one_adj_rbst, an_average_pn1_rbst</t>
   </si>
   <si>
     <t xml:space="preserve">She saw a owl.</t>
@@ -181,7 +181,7 @@
     <t xml:space="preserve">Apparently by accident, the student's answer contains a doubled word.</t>
   </si>
   <si>
-    <t xml:space="preserve">n_-_pr-he_le_rbst, n_-_pr-she_le_rbst, n_-_pr-it_le_rbst, n_-_pr-they_le_rbst, n_-_pr-i_le_rbst, n_-_pr-we_le_rbst, n_-_pr-you_le_rbst, her_poss_stutter_rbst, his_poss_stutter_rbst, its_poss_stutter_rbst, my_poss_stutter_rbst, our_poss_stutter_rbst, your_poss_stutter_rbst, their_poss_stutter_rbst, and_conj_stutter_rbst, but_conj_stutter_rbst, or_conj_stutter_rbst, p_np_i-nm-poss_le_rbst, to_c_prop_stutter_rbst, to_p_stutter_rbst, n_-_pr-he_le_rbst, n_-_pr-i_le_rbst, n_-_pr-it_le_rbst, n_-_pr-she_le_rbst, n_-_pr-they_le_rbst, n_-_pr-we_le_rbst, n_-_pr-you_le_rbst, a_a_det_rbst, an_an_det_1_rbst, an_det_2_rbst, a_det_3_rbst, the_2_rbst, the_3_rbst, the_5_rbst, an_an_det_1_rbst, an_an_det_1b_rbst, an_an_det_1c_rbst, an_det_2_rbst, the_4_rbst, the_6_rbst, the_7_rbst, of_poss_stutter_rbst</t>
+    <t xml:space="preserve">n_-_pr-he_le_rbst, n_-_pr-she_le_rbst, n_-_pr-it_le_rbst, n_-_pr-they_le_rbst, n_-_pr-i_le_rbst, n_-_pr-we_le_rbst, n_-_pr-you_le_rbst, her_poss_stutter_rbst, his_poss_stutter_rbst, its_poss_stutter_rbst, my_poss_stutter_rbst, our_poss_stutter_rbst, your_poss_stutter_rbst, their_poss_stutter_rbst, and_conj_stutter_rbst, but_conj_stutter_rbst, or_conj_stutter_rbst, to_c_prop_stutter_rbst, to_p_stutter_rbst, n_-_pr-he_le_rbst, n_-_pr-i_le_rbst, n_-_pr-it_le_rbst, n_-_pr-she_le_rbst, n_-_pr-they_le_rbst, n_-_pr-we_le_rbst, n_-_pr-you_le_rbst, a_a_det_rbst, an_an_det_1_rbst, an_det_2_rbst, a_det_3_rbst, the_2_rbst, the_3_rbst, the_5_rbst, an_an_det_1_rbst, an_an_det_1b_rbst, an_an_det_1c_rbst, an_det_2_rbst, the_4_rbst, the_6_rbst, the_7_rbst, of_poss_stutter_rbst</t>
   </si>
   <si>
     <t xml:space="preserve">She bought it it in a museum.</t>
@@ -208,7 +208,7 @@
     <t xml:space="preserve">The student's sentence contains a subject/verb agreement problem.</t>
   </si>
   <si>
-    <t xml:space="preserve">third_sg_fin_v_rbst, non_third_sg_fin_v_rbst, plur_noun_irule_rbst, be_th_cop_is_rbst, be_th_cop_are_rbst, be_th_cop_was_rbst, be_th_cop_were_rbst, be_c_is_rbst, be_c_are_rbst, be_c_was_rbst, be_c_were_rbst, do1_pos_sg_rbst, does1_pos_pl_rbst, va_doesnt_neg_pres_le_rbst, va_dont_neg_pres_le_rbst, have_fin_aux_rbst, has_aux_rbst, be_np_is_rbst, be_np_are_rbst, be_np_was_rbst, be_np_were_rbst, v_vp_has-n_le_rbst, v_vp_have-f-n_le_rbst, be_c_is_neg_rbst, be_c_are_neg_rbst, be_c_was_neg_rbst, be_c_were_neg_rbst, v_np-xp_is-n_le_rbst, v_np-xp_are-n_le_rbst, v_np-xp_was-n_le_rbst, v_np-xp_were-n_le_rbst, v_np_are-n_le_rbst, v_np_is-n_le_rbst, v_np_wre-n_le_rbst, v_np_was-n_le_rbst, be_c_is_neg_q_rbst, be_c_is_neg_u_rbst, be_c_are_neg_rbst, be_c_are_neg_q_rbst, be_c_are_neg_u_rbst, be_c_was_neg_q_rbst, be_c_was_neg_u_rbst, be_c_were_neg_q_rbst, be_c_were_neg_u_rbst</t>
+    <t xml:space="preserve">third_sg_fin_v_rbst, non_third_sg_fin_v_rbst, plur_noun_irule_rbst, be_th_cop_is_rbst, be_th_cop_are_rbst, be_th_cop_was_rbst, be_th_cop_were_rbst, be_c_is_rbst, be_c_are_rbst, be_c_was_rbst, be_c_were_rbst, do1_pos_sg_rbst, does1_pos_pl_rbst, va_doesnt_neg_pres_le_rbst, va_dont_neg_pres_le_rbst, have_fin_aux_rbst, has_aux_rbst, be_np_is_rbst, be_np_are_rbst, be_np_was_rbst, be_np_were_rbst, v_vp_has-n_le_rbst, v_vp_have-f-n_le_rbst, be_c_is_neg_rbst, be_c_are_neg_rbst, be_c_was_neg_rbst, be_c_were_neg_rbst, v_np-xp_is-n_le_rbst, v_np-xp_are-n_le_rbst, v_np-xp_was-n_le_rbst, v_np-xp_were-n_le_rbst, v_np_are-n_le_rbst, v_np_is-n_le_rbst, v_np_wre-n_le_rbst, v_np_was-n_le_rbst, be_c_is_neg_q_rbst, be_c_is_neg_u_rbst, be_c_are_neg_rbst, be_c_are_neg_q_rbst, be_c_are_neg_u_rbst, be_c_was_neg_q_rbst, be_c_was_neg_u_rbst, be_c_were_neg_q_rbst, be_c_were_neg_u_rbst, be_th_cop_was_pl_rbst</t>
   </si>
   <si>
     <t xml:space="preserve">Nancy write a letter.</t>
@@ -553,7 +553,7 @@
     <t xml:space="preserve">np-np_crd-im_c_rbst, n-n_crd-im_c_rbst</t>
   </si>
   <si>
-    <t xml:space="preserve">Dogs, cats and mice appeared.</t>
+    <t xml:space="preserve">Dogs, cats and mice disappeared.</t>
   </si>
   <si>
     <t xml:space="preserve">The student uses the past participle in place of the past form.</t>
@@ -739,7 +739,7 @@
     <t xml:space="preserve">v_pst_scomp_olr_rbst, p_cp_s_le_rbst, p_cp_s-notop_le_rbst, p_cp_s-unsp_le_rbst</t>
   </si>
   <si>
-    <t xml:space="preserve">I felt the driver is friendly.</t>
+    <t xml:space="preserve">I suspected the driver is friendly.</t>
   </si>
   <si>
     <t xml:space="preserve">The student leaves a space before a comma, not after.</t>
@@ -1000,6 +1000,9 @@
     <t xml:space="preserve">Li Ming was admitted into Beijing University.</t>
   </si>
   <si>
+    <t xml:space="preserve">The student wrongly uses "looker-ons" instead of "on-lookers".</t>
+  </si>
+  <si>
     <t xml:space="preserve">looker_on_n1_rbst, looker_on_n2_rbst, lookers_on_n1_rbst, lookers_on_n2_rbst, lookers_on_n3_rbst, lookers_on_n4_rbst</t>
   </si>
   <si>
@@ -1081,7 +1084,7 @@
     <t xml:space="preserve">The student uses a main verb modifying adverb before an auxiliary verb.</t>
   </si>
   <si>
-    <t xml:space="preserve">av_-_i-pr-aux_le_rbst</t>
+    <t xml:space="preserve">av_-_i-pr-aux_le_rbst, all_adv1_rbst</t>
   </si>
   <si>
     <t xml:space="preserve">We almost have written twenty compositions.</t>
@@ -1264,6 +1267,9 @@
     <t xml:space="preserve">It is sure that he will succeed.</t>
   </si>
   <si>
+    <t xml:space="preserve">The student uses the infinitival rather than the -ing verb form following "worth".</t>
+  </si>
+  <si>
     <t xml:space="preserve">worth_a1_rbst</t>
   </si>
   <si>
@@ -1393,7 +1399,7 @@
     <t xml:space="preserve">later_and_sooner_adv1_rbst, later_or_sooner_adv1_rbst</t>
   </si>
   <si>
-    <t xml:space="preserve">You will succeed later and sooner.</t>
+    <t xml:space="preserve">You will arrive later and sooner.</t>
   </si>
   <si>
     <t xml:space="preserve">The student pairs “although...” with “but ...”.</t>
@@ -1429,7 +1435,7 @@
     <t xml:space="preserve">pay_for_v1_rbst</t>
   </si>
   <si>
-    <t xml:space="preserve">We will pay for you today.</t>
+    <t xml:space="preserve">He will pay for us today.</t>
   </si>
   <si>
     <t xml:space="preserve">The student uses the wrong preposition with “instead”.</t>
@@ -1465,7 +1471,7 @@
     <t xml:space="preserve">v_np-pp_np_le_rbst</t>
   </si>
   <si>
-    <t xml:space="preserve">That book cost a lot of money from him.</t>
+    <t xml:space="preserve">It is costing too much money from him.</t>
   </si>
   <si>
     <t xml:space="preserve">The student omits the final “s” on “follows”.</t>
@@ -1501,7 +1507,7 @@
     <t xml:space="preserve">take_adv_rbst</t>
   </si>
   <si>
-    <t xml:space="preserve">We mustn’t take them light.</t>
+    <t xml:space="preserve">He took them very serious.</t>
   </si>
   <si>
     <t xml:space="preserve">The student uses a noun instead of the verb.</t>
@@ -1558,13 +1564,22 @@
     <t xml:space="preserve">She will propose that he leaves.</t>
   </si>
   <si>
+    <t xml:space="preserve">The student omits the matching right comma in apposition.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hdn-np_app-rbc_c_rbst, hdn-np_app-idf-rbc_c_rbst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">His brother, the plumber arrived.</t>
+  </si>
+  <si>
     <t xml:space="preserve">The student uses the wrong form of the verb.</t>
   </si>
   <si>
     <t xml:space="preserve">than_vp_p1_rbst,  aj_vp_inf-prp_olr_rbst, v_vp_ssr-prp_le_rbst</t>
   </si>
   <si>
-    <t xml:space="preserve">It is better to laugh than crying.</t>
+    <t xml:space="preserve">It is better to laugh than weeping.</t>
   </si>
   <si>
     <t xml:space="preserve">The student uses active rather than passive voice for resultative.</t>
@@ -1645,7 +1660,7 @@
     <t xml:space="preserve">be_nv_is_rbst, be_nv_are_rbst, be_nv_been_rbst, be_nv_be_rbst, be_nv_being_rbst, be_nv_was_rbst, be_nv_were_rbst</t>
   </si>
   <si>
-    <t xml:space="preserve">My suggestion is we try again.</t>
+    <t xml:space="preserve">My suggestion is we try it again.</t>
   </si>
   <si>
     <t xml:space="preserve">The student uses subj-aux inversion for an embedded clause.</t>
@@ -1654,7 +1669,7 @@
     <t xml:space="preserve">cl_np-wh_c_rbst</t>
   </si>
   <si>
-    <t xml:space="preserve">What will he say should surprise them.</t>
+    <t xml:space="preserve">What will he do should surprise them.</t>
   </si>
   <si>
     <t xml:space="preserve">The student uses informal “till” instead of “until”.</t>
@@ -1690,7 +1705,7 @@
     <t xml:space="preserve">where_rel_np_rbst, when_rel_np_rbst</t>
   </si>
   <si>
-    <t xml:space="preserve">The place where we saw was beautiful.</t>
+    <t xml:space="preserve">The place where we took pictures of was beautiful.</t>
   </si>
   <si>
     <t xml:space="preserve">The student uses “is” instead of “am”.</t>
@@ -1741,7 +1756,7 @@
     <t xml:space="preserve">The student forms a compound with non-head “time”.</t>
   </si>
   <si>
-    <t xml:space="preserve">time_cmpd_n1_rbst</t>
+    <t xml:space="preserve">first_time_n1_rbst, second_time_n1_rbst, third_time_n1_rbst</t>
   </si>
   <si>
     <t xml:space="preserve">That was my second time win.</t>
@@ -1753,7 +1768,7 @@
     <t xml:space="preserve">once_in_p_rbst</t>
   </si>
   <si>
-    <t xml:space="preserve">We have coffee once in a day.</t>
+    <t xml:space="preserve">Once in a day, we have coffee.</t>
   </si>
   <si>
     <t xml:space="preserve">The student adds a spurious “all”.</t>
@@ -1783,15 +1798,6 @@
     <t xml:space="preserve">the cat slept.</t>
   </si>
   <si>
-    <t xml:space="preserve">The student omits the matching right comma in apposition.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hdn-np_app-rbc_c_rbst, hdn-np_app-idf-rbc_c_rbst</t>
-  </si>
-  <si>
-    <t xml:space="preserve">His brother, the plumber arrived.</t>
-  </si>
-  <si>
     <t xml:space="preserve">The student may be overusing topicalization.</t>
   </si>
   <si>
@@ -1822,10 +1828,439 @@
     <t xml:space="preserve">The student replaces there-copula with `have’.</t>
   </si>
   <si>
-    <t xml:space="preserve">be_th_cop_is_has_rbst, be_th_cop_are_have_rbst, be_th_cop_was_had_rbst, be_th_cop_were_had_rbst</t>
+    <t xml:space="preserve">be_th_cop_is_has_rbst, be_th_cop_are_have_rbst, be_th_cop_was_had_rbst, be_th_cop_were_had_rbst, be_th_cop_be_have_rbst</t>
   </si>
   <si>
     <t xml:space="preserve">There have many solutions for this problem.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The student uses an incorrect form of the reflexive pronoun.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hisself_rbst, hisself_adv_rbst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">He admired hisself.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ourself_rbst, ourself_adv_rbst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We admired ourself.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The student uses double marking of plural possessive.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">apostrophe_s_pl_rbst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The teachers's students arrived.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The student omits "the" before "same".</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aj_pp_i-cmp-sme_le_rbst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We had same answers.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The student uses indicative instead of subjunctive verb form.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if_i_was_you_pre_rbst, if_I_was_you_post_rbst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If I was you, I would work harder.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The student adds a spurious "the" with an abstract noun.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nature_n1_rbst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We enjoyed the beauty of the nature.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The student uses the wrong productive plural form of a noun.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n_pl-reg_olr_rbst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">They live in citys.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The student uses the wrong plural form for "passer by".</t>
+  </si>
+  <si>
+    <t xml:space="preserve">passers_by_n1_rbst, passers_by_n2_rbst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The passer bys were surprised.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The student adds a spurious article for an idiomatic expression.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">in_a_fact_adv1_rbst, in_a_fact_adv2_rbst, in_a_fact_adv3_rbst, in_the_fact_adv1_rbst, in_the_fact_adv2_rbst, in_the_fact_adv3_rbst, at_heart_adv_rbst, by_heart_adv_rbst, to_heart_adv_rbst, by_hand_adv1_rbst, at_heart_adv_rbst, at_temp_rbst, at_first_adv1_rbst, at_last_adv2_rbst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In a fact, we were all late.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The student omits "the" in a partitive phrase.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">det_prt-indef_dlr_rbst, det_prt-of-nagr_dlr_rbst, half_n1_rbst, num_prt-of-def_c_rbst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All of money had disappeared. Each of my toy broke.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The student uses no marking or the wrong form for possessive of irregular plural NP.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">people_n1_poss_rbst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The people money was all spent.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The student adds a spurious "a/an" with "no such".</t>
+  </si>
+  <si>
+    <t xml:space="preserve">such_a_a1_rbst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">He said no such a thing.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The student wrongly inflects a degree measure nominal used with an attributive adjective</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mnp_deg-attr_c_rbst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The two feet tall fence appeared.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The student wrongly fails to inflect a degree measure nominal used with a predicative adjective.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mnp_deg-prd_c_rbst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The fence was two foot tall.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The student has a number mismatch of NPs with identity copula.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">be_id_is_rbst, be_id_is_neg_rbst, be_id_was_rbst, be_id_was_neg_rbst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">My friend is the neighbors.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The student wrongly uses a singular noun in a fixed plural expression.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n_-_c-sg_le_rbst, n_-_c-sg-nonnom_le_rbst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">She expressed her thank.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The student wrongly uses a verb in place of the cognate noun.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">begin_beginning_rbst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We heard the begin section.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The student wrongly inserts one or more articles in this idiom.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">last+but+not+least_adv1_rbst, last+but+not+least_adv2_rbst, last+but+not+least_adv3_rbst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">And the last but not the least, we won.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The student wrongly inserts an article in this idiom.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">first_of_all_adv1_rbst, first_of_all_adv2_rbst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">But the first of all, we won.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The student confuses nominative for possessive pronoun.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">your_you_rbst, your_yourself_rbst, our_we_rbst, their_they_rbst, their_themselves_rbst, my_me_rbst, my_myself_rbst, its_itself_poss_rbst, his_himself_poss_rbst, her_herself_poss_rbst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">He lost you book.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The student confuses possessive for nominative pronoun.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">they_their_rbst, we_our_rbst, you_your_rbst, my_mine_rbst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Our went to the museum.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The student confuses possessive for object pronoun.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">us_our_rbst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">She gave our a book.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The student confuses the free possessive with the bound possessive form.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">our_ours_rbst, our_our_s_rbst, your_yours_rbst, hers_her_poss_rbst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ours book is new.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The student confuses the degree measure modifier for count vs. mass noun.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a+few_little_det_rbst, a+little_few_a1_rbst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We had a few rain today.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The student confuses "another" for "other".</t>
+  </si>
+  <si>
+    <t xml:space="preserve">another_other_a1_rbst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In another words, we lost.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The student wrongly orders a pronoun object with the particle.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">v_pron-prtcl_dlr_rbst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">She picked up it.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The student wrongly uses the plural form of "something".</t>
+  </si>
+  <si>
+    <t xml:space="preserve">somethings_rbst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We found somethings.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The student misspells the second person reflexive.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yourself_youself_rbst, yourself_youself_adv_rbst, yourselves_youselves_rbst, yourselves_youselves_adv_rbst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You can do it youself.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The student misspells the idiomatic phrase.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yours_truly_rbst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your truly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The student confuses the reflexive form for the nominative pronoun.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">he_himself_rbst, she_herself_rbst, it_itself_rbst, i_myself_rbst, you_yourself_rbst, we_ourself_rbst, we_ourselves_rbst, they_themself_rbst, they_themselves_rbst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Himself is winning.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The student confuses a reflexive form for the possessive.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">her_herselfs_poss_rbst, his_himselfs_poss_rbst, its_itselfs_poss_rbst, my_myselfs_rbst, our_ourselves_rbst, our_ourselves2_rbst, their_themselfs_rbst, their_themselves_rbst, your_yourselfs_rbst, your_yourselves_rbst, our_ourselfs_rbst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We lost ourselves's books.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The student wrongly orders "else" before its target.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">else_deg_rbst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">They didn't buy else anything.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The student confuses "none" for "no".</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no_none_det_rbst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We have none books.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The student omits subject-verb number agreement with inverted locative "be".</t>
+  </si>
+  <si>
+    <t xml:space="preserve">be_inv_are_is_rbst, be_inv_is_are_rbst, be_inv_was_were_rbst, be_inv_were_was_rbst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">On the table is some books.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The student wrongly spells the adverb "fast" as "fastly".</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fastly_adv1_rbst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">She moved fastly.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The student wrongly spells "supposed (to)" as "suppose".</t>
+  </si>
+  <si>
+    <t xml:space="preserve">supposed_a2_rbst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We are suppose to disappear.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The student omits the preposition for the adjective's complement.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aj_np_i_le_rbst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">He is very close the desk.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The student confuses temporal "on" for "at".</t>
+  </si>
+  <si>
+    <t xml:space="preserve">on_at_temp_rbst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We began on 2pm.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The student confuses temporal "on" for "in" with months or years.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">on_at_temp_2_rbst, on_at_temp_3_rbst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We began on October.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The student wrongly uses the passive with active argument roles.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">improve_psv_v1_rbst, increased_v2_rbst, decreased_v1_rbst, increase_psv_np_rbst, decrease_psv_np_rbst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">They are improved their situation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The student wrongly uses a plural measure phrase in a compound.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n-hdn_cpd-mnp_c_rbst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">They moved the ten tons rock.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The student confuses “mine” for “my”.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mine_my_rbst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mine book disappeared.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The student wrongly uses a plural noun after "per".</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p_nb_i_le_rbst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">They charged ten cents per children.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The student uses the wrong preposition in an idiomatic expression</t>
+  </si>
+  <si>
+    <t xml:space="preserve">by_this_way_adv_rbst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">By this way, we can make progress.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The student uses emphatic "do" unintentionally.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">did1_pos_rbst, does1_pos_rbst, do1_pos_rbst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The children do play in the park.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The student wrongly omits a comma after a discourse connective.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">last_adv_rbst, third_adv_rbst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Third, we should sleep.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The student omits an obligatory expletive "it" object. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">v_prd_seq_le_rbst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">They made easier to win.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The student wrongly uses a finite clausal complement with "opportunity" rather than an infinitival VP.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">opportunity_n4_rbst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We have an opportunity that we sleep.</t>
   </si>
 </sst>
 </file>
@@ -1835,7 +2270,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1874,6 +2309,12 @@
     <font>
       <sz val="10"/>
       <name val="Noto sans cjk sc regular"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Cambria"/>
       <family val="0"/>
       <charset val="1"/>
     </font>
@@ -1941,7 +2382,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1964,6 +2405,10 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -2043,10 +2488,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T207"/>
+  <dimension ref="A1:T255"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A194" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C206" activeCellId="0" sqref="C206"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5225,12 +5670,14 @@
       <c r="T113" s="2"/>
     </row>
     <row r="114" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A114" s="2"/>
+      <c r="A114" s="2" t="s">
+        <v>325</v>
+      </c>
       <c r="B114" s="2" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="D114" s="2"/>
       <c r="E114" s="2"/>
@@ -5252,13 +5699,13 @@
     </row>
     <row r="115" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A115" s="2" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="D115" s="2"/>
       <c r="E115" s="2"/>
@@ -5280,13 +5727,13 @@
     </row>
     <row r="116" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A116" s="2" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D116" s="2"/>
       <c r="E116" s="2"/>
@@ -5308,13 +5755,13 @@
     </row>
     <row r="117" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A117" s="2" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="D117" s="2"/>
       <c r="E117" s="2"/>
@@ -5336,13 +5783,13 @@
     </row>
     <row r="118" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A118" s="2" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D118" s="2"/>
       <c r="E118" s="2"/>
@@ -5364,13 +5811,13 @@
     </row>
     <row r="119" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A119" s="2" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="D119" s="2"/>
       <c r="E119" s="2"/>
@@ -5392,13 +5839,13 @@
     </row>
     <row r="120" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A120" s="2" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="D120" s="2"/>
       <c r="E120" s="2"/>
@@ -5420,13 +5867,13 @@
     </row>
     <row r="121" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A121" s="2" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="D121" s="2"/>
       <c r="E121" s="2"/>
@@ -5448,13 +5895,13 @@
     </row>
     <row r="122" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A122" s="2" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="D122" s="2"/>
       <c r="E122" s="2"/>
@@ -5476,13 +5923,13 @@
     </row>
     <row r="123" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A123" s="2" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="D123" s="2"/>
       <c r="E123" s="2"/>
@@ -5504,13 +5951,13 @@
     </row>
     <row r="124" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A124" s="2" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="D124" s="2"/>
       <c r="E124" s="2"/>
@@ -5535,10 +5982,10 @@
         <v>146</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="D125" s="2"/>
       <c r="E125" s="2"/>
@@ -5560,13 +6007,13 @@
     </row>
     <row r="126" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A126" s="2" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="D126" s="2"/>
       <c r="E126" s="2"/>
@@ -5588,13 +6035,13 @@
     </row>
     <row r="127" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A127" s="2" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="D127" s="2"/>
       <c r="E127" s="2"/>
@@ -5616,13 +6063,13 @@
     </row>
     <row r="128" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A128" s="2" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="D128" s="2"/>
       <c r="E128" s="2"/>
@@ -5644,13 +6091,13 @@
     </row>
     <row r="129" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A129" s="2" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="D129" s="2"/>
       <c r="E129" s="2"/>
@@ -5672,13 +6119,13 @@
     </row>
     <row r="130" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A130" s="2" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="D130" s="2"/>
       <c r="E130" s="2"/>
@@ -5700,13 +6147,13 @@
     </row>
     <row r="131" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A131" s="2" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="D131" s="2"/>
       <c r="E131" s="2"/>
@@ -5728,13 +6175,13 @@
     </row>
     <row r="132" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A132" s="2" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="D132" s="2"/>
       <c r="E132" s="2"/>
@@ -5756,13 +6203,13 @@
     </row>
     <row r="133" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A133" s="2" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="D133" s="2"/>
       <c r="E133" s="2"/>
@@ -5784,13 +6231,13 @@
     </row>
     <row r="134" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A134" s="2" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="D134" s="2"/>
       <c r="E134" s="2"/>
@@ -5812,13 +6259,13 @@
     </row>
     <row r="135" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A135" s="2" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="D135" s="2"/>
       <c r="E135" s="2"/>
@@ -5840,13 +6287,13 @@
     </row>
     <row r="136" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A136" s="2" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="D136" s="2"/>
       <c r="E136" s="2"/>
@@ -5868,13 +6315,13 @@
     </row>
     <row r="137" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A137" s="2" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="D137" s="2"/>
       <c r="E137" s="2"/>
@@ -5896,13 +6343,13 @@
     </row>
     <row r="138" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A138" s="2" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D138" s="2"/>
       <c r="E138" s="2"/>
@@ -5924,13 +6371,13 @@
     </row>
     <row r="139" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A139" s="2" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="D139" s="2"/>
       <c r="E139" s="2"/>
@@ -5952,13 +6399,13 @@
     </row>
     <row r="140" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A140" s="2" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="D140" s="2"/>
       <c r="E140" s="2"/>
@@ -5980,13 +6427,13 @@
     </row>
     <row r="141" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A141" s="2" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="D141" s="2"/>
       <c r="E141" s="2"/>
@@ -6008,13 +6455,13 @@
     </row>
     <row r="142" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A142" s="2" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="D142" s="2"/>
       <c r="E142" s="2"/>
@@ -6036,13 +6483,13 @@
     </row>
     <row r="143" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A143" s="2" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="D143" s="2"/>
       <c r="E143" s="2"/>
@@ -6063,12 +6510,14 @@
       <c r="T143" s="2"/>
     </row>
     <row r="144" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A144" s="2"/>
+      <c r="A144" s="2" t="s">
+        <v>414</v>
+      </c>
       <c r="B144" s="2" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="D144" s="2"/>
       <c r="E144" s="2"/>
@@ -6090,13 +6539,13 @@
     </row>
     <row r="145" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A145" s="2" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="D145" s="2"/>
       <c r="E145" s="2"/>
@@ -6118,13 +6567,13 @@
     </row>
     <row r="146" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A146" s="2" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="D146" s="2"/>
       <c r="E146" s="2"/>
@@ -6146,13 +6595,13 @@
     </row>
     <row r="147" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A147" s="2" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="D147" s="2"/>
       <c r="E147" s="2"/>
@@ -6174,13 +6623,13 @@
     </row>
     <row r="148" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A148" s="2" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="D148" s="2"/>
       <c r="E148" s="2"/>
@@ -6202,13 +6651,13 @@
     </row>
     <row r="149" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A149" s="2" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="D149" s="2"/>
       <c r="E149" s="2"/>
@@ -6230,13 +6679,13 @@
     </row>
     <row r="150" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A150" s="2" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="D150" s="2"/>
       <c r="E150" s="2"/>
@@ -6258,13 +6707,13 @@
     </row>
     <row r="151" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A151" s="2" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="D151" s="2"/>
       <c r="E151" s="2"/>
@@ -6286,13 +6735,13 @@
     </row>
     <row r="152" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A152" s="2" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="D152" s="2"/>
       <c r="E152" s="2"/>
@@ -6314,13 +6763,13 @@
     </row>
     <row r="153" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A153" s="2" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="D153" s="2"/>
       <c r="E153" s="2"/>
@@ -6342,13 +6791,13 @@
     </row>
     <row r="154" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A154" s="2" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="D154" s="2"/>
       <c r="E154" s="2"/>
@@ -6370,13 +6819,13 @@
     </row>
     <row r="155" customFormat="false" ht="48.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A155" s="2" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="D155" s="2"/>
       <c r="E155" s="2"/>
@@ -6398,13 +6847,13 @@
     </row>
     <row r="156" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A156" s="2" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="D156" s="2"/>
       <c r="E156" s="2"/>
@@ -6426,13 +6875,13 @@
     </row>
     <row r="157" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A157" s="2" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="D157" s="2"/>
       <c r="E157" s="2"/>
@@ -6454,13 +6903,13 @@
     </row>
     <row r="158" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A158" s="2" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="D158" s="2"/>
       <c r="E158" s="2"/>
@@ -6482,13 +6931,13 @@
     </row>
     <row r="159" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A159" s="2" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="D159" s="2"/>
       <c r="E159" s="2"/>
@@ -6510,13 +6959,13 @@
     </row>
     <row r="160" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A160" s="2" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="D160" s="2"/>
       <c r="E160" s="2"/>
@@ -6538,13 +6987,13 @@
     </row>
     <row r="161" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A161" s="2" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="D161" s="2"/>
       <c r="E161" s="2"/>
@@ -6566,13 +7015,13 @@
     </row>
     <row r="162" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A162" s="2" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="D162" s="2"/>
       <c r="E162" s="2"/>
@@ -6594,13 +7043,13 @@
     </row>
     <row r="163" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A163" s="2" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="D163" s="2"/>
       <c r="E163" s="2"/>
@@ -6622,13 +7071,13 @@
     </row>
     <row r="164" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A164" s="2" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="D164" s="2"/>
       <c r="E164" s="2"/>
@@ -6650,13 +7099,13 @@
     </row>
     <row r="165" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A165" s="2" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="D165" s="2"/>
       <c r="E165" s="2"/>
@@ -6678,13 +7127,13 @@
     </row>
     <row r="166" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A166" s="2" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="D166" s="2"/>
       <c r="E166" s="2"/>
@@ -6706,13 +7155,13 @@
     </row>
     <row r="167" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A167" s="2" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="D167" s="2"/>
       <c r="E167" s="2"/>
@@ -6734,13 +7183,13 @@
     </row>
     <row r="168" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A168" s="2" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="D168" s="2"/>
       <c r="E168" s="2"/>
@@ -6762,13 +7211,13 @@
     </row>
     <row r="169" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A169" s="2" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="D169" s="2"/>
       <c r="E169" s="2"/>
@@ -6790,13 +7239,13 @@
     </row>
     <row r="170" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A170" s="2" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="D170" s="2"/>
       <c r="E170" s="2"/>
@@ -6818,13 +7267,13 @@
     </row>
     <row r="171" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A171" s="2" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="D171" s="2"/>
       <c r="E171" s="2"/>
@@ -6846,13 +7295,13 @@
     </row>
     <row r="172" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A172" s="2" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="D172" s="2"/>
       <c r="E172" s="2"/>
@@ -6874,13 +7323,13 @@
     </row>
     <row r="173" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A173" s="2" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="D173" s="2"/>
       <c r="E173" s="2"/>
@@ -6902,13 +7351,13 @@
     </row>
     <row r="174" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A174" s="2" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="D174" s="2"/>
       <c r="E174" s="2"/>
@@ -6930,13 +7379,13 @@
     </row>
     <row r="175" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A175" s="2" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="D175" s="2"/>
       <c r="E175" s="2"/>
@@ -6958,13 +7407,13 @@
     </row>
     <row r="176" customFormat="false" ht="73.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A176" s="2" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="D176" s="2"/>
       <c r="E176" s="2"/>
@@ -6984,15 +7433,15 @@
       <c r="S176" s="2"/>
       <c r="T176" s="2"/>
     </row>
-    <row r="177" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A177" s="2" t="s">
-        <v>511</v>
-      </c>
-      <c r="B177" s="2" t="s">
-        <v>512</v>
-      </c>
-      <c r="C177" s="2" t="s">
+    <row r="177" customFormat="false" ht="73.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A177" s="6" t="s">
         <v>513</v>
+      </c>
+      <c r="B177" s="6" t="s">
+        <v>514</v>
+      </c>
+      <c r="C177" s="6" t="s">
+        <v>515</v>
       </c>
       <c r="D177" s="2"/>
       <c r="E177" s="2"/>
@@ -7012,15 +7461,15 @@
       <c r="S177" s="2"/>
       <c r="T177" s="2"/>
     </row>
-    <row r="178" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="178" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A178" s="2" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="D178" s="2"/>
       <c r="E178" s="2"/>
@@ -7040,15 +7489,15 @@
       <c r="S178" s="2"/>
       <c r="T178" s="2"/>
     </row>
-    <row r="179" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="179" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A179" s="2" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="D179" s="2"/>
       <c r="E179" s="2"/>
@@ -7068,15 +7517,15 @@
       <c r="S179" s="2"/>
       <c r="T179" s="2"/>
     </row>
-    <row r="180" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="180" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A180" s="2" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="D180" s="2"/>
       <c r="E180" s="2"/>
@@ -7098,13 +7547,13 @@
     </row>
     <row r="181" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A181" s="2" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>524</v>
+        <v>526</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="D181" s="2"/>
       <c r="E181" s="2"/>
@@ -7124,15 +7573,15 @@
       <c r="S181" s="2"/>
       <c r="T181" s="2"/>
     </row>
-    <row r="182" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="182" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A182" s="2" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="D182" s="2"/>
       <c r="E182" s="2"/>
@@ -7154,13 +7603,13 @@
     </row>
     <row r="183" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A183" s="2" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="C183" s="2" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="D183" s="2"/>
       <c r="E183" s="2"/>
@@ -7182,13 +7631,13 @@
     </row>
     <row r="184" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A184" s="2" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>533</v>
+        <v>535</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="D184" s="2"/>
       <c r="E184" s="2"/>
@@ -7208,15 +7657,15 @@
       <c r="S184" s="2"/>
       <c r="T184" s="2"/>
     </row>
-    <row r="185" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="185" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A185" s="2" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="C185" s="2" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="D185" s="2"/>
       <c r="E185" s="2"/>
@@ -7238,13 +7687,13 @@
     </row>
     <row r="186" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A186" s="2" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="D186" s="2"/>
       <c r="E186" s="2"/>
@@ -7266,13 +7715,13 @@
     </row>
     <row r="187" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A187" s="2" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
       <c r="D187" s="2"/>
       <c r="E187" s="2"/>
@@ -7294,13 +7743,13 @@
     </row>
     <row r="188" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A188" s="2" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
       <c r="C188" s="2" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="D188" s="2"/>
       <c r="E188" s="2"/>
@@ -7320,15 +7769,15 @@
       <c r="S188" s="2"/>
       <c r="T188" s="2"/>
     </row>
-    <row r="189" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="189" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A189" s="2" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="C189" s="2" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="D189" s="2"/>
       <c r="E189" s="2"/>
@@ -7350,13 +7799,13 @@
     </row>
     <row r="190" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A190" s="2" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>551</v>
+        <v>553</v>
       </c>
       <c r="C190" s="2" t="s">
-        <v>552</v>
+        <v>554</v>
       </c>
       <c r="D190" s="2"/>
       <c r="E190" s="2"/>
@@ -7376,15 +7825,15 @@
       <c r="S190" s="2"/>
       <c r="T190" s="2"/>
     </row>
-    <row r="191" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="191" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A191" s="2" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
       <c r="C191" s="2" t="s">
-        <v>555</v>
+        <v>557</v>
       </c>
       <c r="D191" s="2"/>
       <c r="E191" s="2"/>
@@ -7404,15 +7853,15 @@
       <c r="S191" s="2"/>
       <c r="T191" s="2"/>
     </row>
-    <row r="192" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="192" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A192" s="2" t="s">
-        <v>556</v>
+        <v>558</v>
       </c>
       <c r="B192" s="2" t="s">
-        <v>557</v>
+        <v>559</v>
       </c>
       <c r="C192" s="2" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="D192" s="2"/>
       <c r="E192" s="2"/>
@@ -7434,13 +7883,13 @@
     </row>
     <row r="193" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A193" s="2" t="s">
-        <v>559</v>
+        <v>561</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="C193" s="2" t="s">
-        <v>561</v>
+        <v>563</v>
       </c>
       <c r="D193" s="2"/>
       <c r="E193" s="2"/>
@@ -7460,15 +7909,15 @@
       <c r="S193" s="2"/>
       <c r="T193" s="2"/>
     </row>
-    <row r="194" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="194" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A194" s="2" t="s">
-        <v>562</v>
+        <v>564</v>
       </c>
       <c r="B194" s="2" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
       <c r="C194" s="2" t="s">
-        <v>564</v>
+        <v>566</v>
       </c>
       <c r="D194" s="2"/>
       <c r="E194" s="2"/>
@@ -7490,13 +7939,13 @@
     </row>
     <row r="195" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A195" s="2" t="s">
-        <v>565</v>
+        <v>567</v>
       </c>
       <c r="B195" s="2" t="s">
-        <v>566</v>
+        <v>568</v>
       </c>
       <c r="C195" s="2" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
       <c r="D195" s="2"/>
       <c r="E195" s="2"/>
@@ -7518,13 +7967,13 @@
     </row>
     <row r="196" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A196" s="2" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
       <c r="B196" s="2" t="s">
-        <v>569</v>
+        <v>571</v>
       </c>
       <c r="C196" s="2" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
       <c r="D196" s="2"/>
       <c r="E196" s="2"/>
@@ -7546,13 +7995,13 @@
     </row>
     <row r="197" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A197" s="2" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
       <c r="B197" s="2" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
       <c r="C197" s="2" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="D197" s="2"/>
       <c r="E197" s="2"/>
@@ -7572,15 +8021,15 @@
       <c r="S197" s="2"/>
       <c r="T197" s="2"/>
     </row>
-    <row r="198" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="198" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A198" s="2" t="s">
-        <v>574</v>
+        <v>576</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>575</v>
+        <v>577</v>
       </c>
       <c r="C198" s="2" t="s">
-        <v>576</v>
+        <v>578</v>
       </c>
       <c r="D198" s="2"/>
       <c r="E198" s="2"/>
@@ -7600,15 +8049,15 @@
       <c r="S198" s="2"/>
       <c r="T198" s="2"/>
     </row>
-    <row r="199" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="199" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A199" s="2" t="s">
-        <v>577</v>
+        <v>579</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>578</v>
+        <v>580</v>
       </c>
       <c r="C199" s="2" t="s">
-        <v>579</v>
+        <v>581</v>
       </c>
       <c r="D199" s="2"/>
       <c r="E199" s="2"/>
@@ -7630,13 +8079,13 @@
     </row>
     <row r="200" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A200" s="2" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
       <c r="B200" s="2" t="s">
-        <v>581</v>
+        <v>583</v>
       </c>
       <c r="C200" s="2" t="s">
-        <v>582</v>
+        <v>584</v>
       </c>
       <c r="D200" s="2"/>
       <c r="E200" s="2"/>
@@ -7658,13 +8107,13 @@
     </row>
     <row r="201" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A201" s="2" t="s">
-        <v>583</v>
+        <v>585</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="C201" s="2" t="s">
-        <v>585</v>
+        <v>587</v>
       </c>
       <c r="D201" s="2"/>
       <c r="E201" s="2"/>
@@ -7686,13 +8135,13 @@
     </row>
     <row r="202" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A202" s="2" t="s">
-        <v>586</v>
+        <v>588</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>587</v>
+        <v>589</v>
       </c>
       <c r="C202" s="2" t="s">
-        <v>588</v>
+        <v>590</v>
       </c>
       <c r="D202" s="2"/>
       <c r="E202" s="2"/>
@@ -7714,13 +8163,13 @@
     </row>
     <row r="203" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A203" s="2" t="s">
-        <v>589</v>
+        <v>591</v>
       </c>
       <c r="B203" s="2" t="s">
-        <v>590</v>
+        <v>592</v>
       </c>
       <c r="C203" s="2" t="s">
-        <v>591</v>
+        <v>593</v>
       </c>
       <c r="D203" s="2"/>
       <c r="E203" s="2"/>
@@ -7742,13 +8191,13 @@
     </row>
     <row r="204" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A204" s="2" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
       <c r="B204" s="2" t="s">
-        <v>593</v>
+        <v>595</v>
       </c>
       <c r="C204" s="2" t="s">
-        <v>594</v>
+        <v>596</v>
       </c>
       <c r="D204" s="2"/>
       <c r="E204" s="2"/>
@@ -7770,13 +8219,13 @@
     </row>
     <row r="205" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A205" s="2" t="s">
-        <v>595</v>
+        <v>597</v>
       </c>
       <c r="B205" s="2" t="s">
-        <v>596</v>
+        <v>598</v>
       </c>
       <c r="C205" s="2" t="s">
-        <v>597</v>
+        <v>599</v>
       </c>
       <c r="D205" s="2"/>
       <c r="E205" s="2"/>
@@ -7798,13 +8247,13 @@
     </row>
     <row r="206" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A206" s="2" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
       <c r="B206" s="2" t="s">
-        <v>599</v>
+        <v>601</v>
       </c>
       <c r="C206" s="2" t="s">
-        <v>600</v>
+        <v>602</v>
       </c>
       <c r="D206" s="2"/>
       <c r="E206" s="2"/>
@@ -7824,54 +8273,1350 @@
       <c r="S206" s="2"/>
       <c r="T206" s="2"/>
     </row>
-    <row r="207" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="208" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="209" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="210" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="211" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="212" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="213" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="214" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="215" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="216" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="217" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="218" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="219" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="220" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="221" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="222" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="223" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="224" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="225" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="226" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="227" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="228" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="229" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="230" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="231" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="232" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="233" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="234" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="235" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="236" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="237" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="238" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="239" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="240" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="241" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="242" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="243" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="244" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="245" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="246" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="247" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="248" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="249" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="250" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="251" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="252" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="253" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="254" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="207" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A207" s="2" t="s">
+        <v>603</v>
+      </c>
+      <c r="B207" s="2" t="s">
+        <v>604</v>
+      </c>
+      <c r="C207" s="2" t="s">
+        <v>605</v>
+      </c>
+      <c r="D207" s="2"/>
+      <c r="E207" s="2"/>
+      <c r="F207" s="2"/>
+      <c r="G207" s="2"/>
+      <c r="H207" s="2"/>
+      <c r="I207" s="2"/>
+      <c r="J207" s="2"/>
+      <c r="K207" s="2"/>
+      <c r="L207" s="2"/>
+      <c r="M207" s="2"/>
+      <c r="N207" s="2"/>
+      <c r="O207" s="2"/>
+      <c r="P207" s="2"/>
+      <c r="Q207" s="2"/>
+      <c r="R207" s="2"/>
+      <c r="S207" s="2"/>
+      <c r="T207" s="2"/>
+    </row>
+    <row r="208" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A208" s="2" t="s">
+        <v>603</v>
+      </c>
+      <c r="B208" s="2" t="s">
+        <v>606</v>
+      </c>
+      <c r="C208" s="2" t="s">
+        <v>607</v>
+      </c>
+      <c r="D208" s="2"/>
+      <c r="E208" s="2"/>
+      <c r="F208" s="2"/>
+      <c r="G208" s="2"/>
+      <c r="H208" s="2"/>
+      <c r="I208" s="2"/>
+      <c r="J208" s="2"/>
+      <c r="K208" s="2"/>
+      <c r="L208" s="2"/>
+      <c r="M208" s="2"/>
+      <c r="N208" s="2"/>
+      <c r="O208" s="2"/>
+      <c r="P208" s="2"/>
+      <c r="Q208" s="2"/>
+      <c r="R208" s="2"/>
+      <c r="S208" s="2"/>
+      <c r="T208" s="2"/>
+    </row>
+    <row r="209" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A209" s="2" t="s">
+        <v>608</v>
+      </c>
+      <c r="B209" s="2" t="s">
+        <v>609</v>
+      </c>
+      <c r="C209" s="2" t="s">
+        <v>610</v>
+      </c>
+      <c r="D209" s="2"/>
+      <c r="E209" s="2"/>
+      <c r="F209" s="2"/>
+      <c r="G209" s="2"/>
+      <c r="H209" s="2"/>
+      <c r="I209" s="2"/>
+      <c r="J209" s="2"/>
+      <c r="K209" s="2"/>
+      <c r="L209" s="2"/>
+      <c r="M209" s="2"/>
+      <c r="N209" s="2"/>
+      <c r="O209" s="2"/>
+      <c r="P209" s="2"/>
+      <c r="Q209" s="2"/>
+      <c r="R209" s="2"/>
+      <c r="S209" s="2"/>
+      <c r="T209" s="2"/>
+    </row>
+    <row r="210" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A210" s="2" t="s">
+        <v>611</v>
+      </c>
+      <c r="B210" s="2" t="s">
+        <v>612</v>
+      </c>
+      <c r="C210" s="2" t="s">
+        <v>613</v>
+      </c>
+      <c r="D210" s="2"/>
+      <c r="E210" s="2"/>
+      <c r="F210" s="2"/>
+      <c r="G210" s="2"/>
+      <c r="H210" s="2"/>
+      <c r="I210" s="2"/>
+      <c r="J210" s="2"/>
+      <c r="K210" s="2"/>
+      <c r="L210" s="2"/>
+      <c r="M210" s="2"/>
+      <c r="N210" s="2"/>
+      <c r="O210" s="2"/>
+      <c r="P210" s="2"/>
+      <c r="Q210" s="2"/>
+      <c r="R210" s="2"/>
+      <c r="S210" s="2"/>
+      <c r="T210" s="2"/>
+    </row>
+    <row r="211" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A211" s="2" t="s">
+        <v>614</v>
+      </c>
+      <c r="B211" s="2" t="s">
+        <v>615</v>
+      </c>
+      <c r="C211" s="2" t="s">
+        <v>616</v>
+      </c>
+      <c r="D211" s="2"/>
+      <c r="E211" s="2"/>
+      <c r="F211" s="2"/>
+      <c r="G211" s="2"/>
+      <c r="H211" s="2"/>
+      <c r="I211" s="2"/>
+      <c r="J211" s="2"/>
+      <c r="K211" s="2"/>
+      <c r="L211" s="2"/>
+      <c r="M211" s="2"/>
+      <c r="N211" s="2"/>
+      <c r="O211" s="2"/>
+      <c r="P211" s="2"/>
+      <c r="Q211" s="2"/>
+      <c r="R211" s="2"/>
+      <c r="S211" s="2"/>
+      <c r="T211" s="2"/>
+    </row>
+    <row r="212" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A212" s="2" t="s">
+        <v>617</v>
+      </c>
+      <c r="B212" s="2" t="s">
+        <v>618</v>
+      </c>
+      <c r="C212" s="2" t="s">
+        <v>619</v>
+      </c>
+      <c r="D212" s="2"/>
+      <c r="E212" s="2"/>
+      <c r="F212" s="2"/>
+      <c r="G212" s="2"/>
+      <c r="H212" s="2"/>
+      <c r="I212" s="2"/>
+      <c r="J212" s="2"/>
+      <c r="K212" s="2"/>
+      <c r="L212" s="2"/>
+      <c r="M212" s="2"/>
+      <c r="N212" s="2"/>
+      <c r="O212" s="2"/>
+      <c r="P212" s="2"/>
+      <c r="Q212" s="2"/>
+      <c r="R212" s="2"/>
+      <c r="S212" s="2"/>
+      <c r="T212" s="2"/>
+    </row>
+    <row r="213" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A213" s="2" t="s">
+        <v>620</v>
+      </c>
+      <c r="B213" s="2" t="s">
+        <v>621</v>
+      </c>
+      <c r="C213" s="2" t="s">
+        <v>622</v>
+      </c>
+      <c r="D213" s="2"/>
+      <c r="E213" s="2"/>
+      <c r="F213" s="2"/>
+      <c r="G213" s="2"/>
+      <c r="H213" s="2"/>
+      <c r="I213" s="2"/>
+      <c r="J213" s="2"/>
+      <c r="K213" s="2"/>
+      <c r="L213" s="2"/>
+      <c r="M213" s="2"/>
+      <c r="N213" s="2"/>
+      <c r="O213" s="2"/>
+      <c r="P213" s="2"/>
+      <c r="Q213" s="2"/>
+      <c r="R213" s="2"/>
+      <c r="S213" s="2"/>
+      <c r="T213" s="2"/>
+    </row>
+    <row r="214" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A214" s="2" t="s">
+        <v>623</v>
+      </c>
+      <c r="B214" s="2" t="s">
+        <v>624</v>
+      </c>
+      <c r="C214" s="2" t="s">
+        <v>625</v>
+      </c>
+      <c r="D214" s="2"/>
+      <c r="E214" s="2"/>
+      <c r="F214" s="2"/>
+      <c r="G214" s="2"/>
+      <c r="H214" s="2"/>
+      <c r="I214" s="2"/>
+      <c r="J214" s="2"/>
+      <c r="K214" s="2"/>
+      <c r="L214" s="2"/>
+      <c r="M214" s="2"/>
+      <c r="N214" s="2"/>
+      <c r="O214" s="2"/>
+      <c r="P214" s="2"/>
+      <c r="Q214" s="2"/>
+      <c r="R214" s="2"/>
+      <c r="S214" s="2"/>
+      <c r="T214" s="2"/>
+    </row>
+    <row r="215" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A215" s="2" t="s">
+        <v>626</v>
+      </c>
+      <c r="B215" s="2" t="s">
+        <v>627</v>
+      </c>
+      <c r="C215" s="2" t="s">
+        <v>628</v>
+      </c>
+      <c r="D215" s="2"/>
+      <c r="E215" s="2"/>
+      <c r="F215" s="2"/>
+      <c r="G215" s="2"/>
+      <c r="H215" s="2"/>
+      <c r="I215" s="2"/>
+      <c r="J215" s="2"/>
+      <c r="K215" s="2"/>
+      <c r="L215" s="2"/>
+      <c r="M215" s="2"/>
+      <c r="N215" s="2"/>
+      <c r="O215" s="2"/>
+      <c r="P215" s="2"/>
+      <c r="Q215" s="2"/>
+      <c r="R215" s="2"/>
+      <c r="S215" s="2"/>
+      <c r="T215" s="2"/>
+    </row>
+    <row r="216" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A216" s="2" t="s">
+        <v>629</v>
+      </c>
+      <c r="B216" s="2" t="s">
+        <v>630</v>
+      </c>
+      <c r="C216" s="2" t="s">
+        <v>631</v>
+      </c>
+      <c r="D216" s="2"/>
+      <c r="E216" s="2"/>
+      <c r="F216" s="2"/>
+      <c r="G216" s="2"/>
+      <c r="H216" s="2"/>
+      <c r="I216" s="2"/>
+      <c r="J216" s="2"/>
+      <c r="K216" s="2"/>
+      <c r="L216" s="2"/>
+      <c r="M216" s="2"/>
+      <c r="N216" s="2"/>
+      <c r="O216" s="2"/>
+      <c r="P216" s="2"/>
+      <c r="Q216" s="2"/>
+      <c r="R216" s="2"/>
+      <c r="S216" s="2"/>
+      <c r="T216" s="2"/>
+    </row>
+    <row r="217" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A217" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="B217" s="2" t="s">
+        <v>633</v>
+      </c>
+      <c r="C217" s="2" t="s">
+        <v>634</v>
+      </c>
+      <c r="D217" s="2"/>
+      <c r="E217" s="2"/>
+      <c r="F217" s="2"/>
+      <c r="G217" s="2"/>
+      <c r="H217" s="2"/>
+      <c r="I217" s="2"/>
+      <c r="J217" s="2"/>
+      <c r="K217" s="2"/>
+      <c r="L217" s="2"/>
+      <c r="M217" s="2"/>
+      <c r="N217" s="2"/>
+      <c r="O217" s="2"/>
+      <c r="P217" s="2"/>
+      <c r="Q217" s="2"/>
+      <c r="R217" s="2"/>
+      <c r="S217" s="2"/>
+      <c r="T217" s="2"/>
+    </row>
+    <row r="218" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A218" s="2" t="s">
+        <v>635</v>
+      </c>
+      <c r="B218" s="2" t="s">
+        <v>636</v>
+      </c>
+      <c r="C218" s="2" t="s">
+        <v>637</v>
+      </c>
+      <c r="D218" s="2"/>
+      <c r="E218" s="2"/>
+      <c r="F218" s="2"/>
+      <c r="G218" s="2"/>
+      <c r="H218" s="2"/>
+      <c r="I218" s="2"/>
+      <c r="J218" s="2"/>
+      <c r="K218" s="2"/>
+      <c r="L218" s="2"/>
+      <c r="M218" s="2"/>
+      <c r="N218" s="2"/>
+      <c r="O218" s="2"/>
+      <c r="P218" s="2"/>
+      <c r="Q218" s="2"/>
+      <c r="R218" s="2"/>
+      <c r="S218" s="2"/>
+      <c r="T218" s="2"/>
+    </row>
+    <row r="219" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A219" s="2" t="s">
+        <v>638</v>
+      </c>
+      <c r="B219" s="2" t="s">
+        <v>639</v>
+      </c>
+      <c r="C219" s="2" t="s">
+        <v>640</v>
+      </c>
+      <c r="D219" s="2"/>
+      <c r="E219" s="2"/>
+      <c r="F219" s="2"/>
+      <c r="G219" s="2"/>
+      <c r="H219" s="2"/>
+      <c r="I219" s="2"/>
+      <c r="J219" s="2"/>
+      <c r="K219" s="2"/>
+      <c r="L219" s="2"/>
+      <c r="M219" s="2"/>
+      <c r="N219" s="2"/>
+      <c r="O219" s="2"/>
+      <c r="P219" s="2"/>
+      <c r="Q219" s="2"/>
+      <c r="R219" s="2"/>
+      <c r="S219" s="2"/>
+      <c r="T219" s="2"/>
+    </row>
+    <row r="220" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A220" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="B220" s="2" t="s">
+        <v>642</v>
+      </c>
+      <c r="C220" s="2" t="s">
+        <v>643</v>
+      </c>
+      <c r="D220" s="2"/>
+      <c r="E220" s="2"/>
+      <c r="F220" s="2"/>
+      <c r="G220" s="2"/>
+      <c r="H220" s="2"/>
+      <c r="I220" s="2"/>
+      <c r="J220" s="2"/>
+      <c r="K220" s="2"/>
+      <c r="L220" s="2"/>
+      <c r="M220" s="2"/>
+      <c r="N220" s="2"/>
+      <c r="O220" s="2"/>
+      <c r="P220" s="2"/>
+      <c r="Q220" s="2"/>
+      <c r="R220" s="2"/>
+      <c r="S220" s="2"/>
+      <c r="T220" s="2"/>
+    </row>
+    <row r="221" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A221" s="2" t="s">
+        <v>644</v>
+      </c>
+      <c r="B221" s="2" t="s">
+        <v>645</v>
+      </c>
+      <c r="C221" s="2" t="s">
+        <v>646</v>
+      </c>
+      <c r="D221" s="2"/>
+      <c r="E221" s="2"/>
+      <c r="F221" s="2"/>
+      <c r="G221" s="2"/>
+      <c r="H221" s="2"/>
+      <c r="I221" s="2"/>
+      <c r="J221" s="2"/>
+      <c r="K221" s="2"/>
+      <c r="L221" s="2"/>
+      <c r="M221" s="2"/>
+      <c r="N221" s="2"/>
+      <c r="O221" s="2"/>
+      <c r="P221" s="2"/>
+      <c r="Q221" s="2"/>
+      <c r="R221" s="2"/>
+      <c r="S221" s="2"/>
+      <c r="T221" s="2"/>
+    </row>
+    <row r="222" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A222" s="2" t="s">
+        <v>647</v>
+      </c>
+      <c r="B222" s="2" t="s">
+        <v>648</v>
+      </c>
+      <c r="C222" s="2" t="s">
+        <v>649</v>
+      </c>
+      <c r="D222" s="2"/>
+      <c r="E222" s="2"/>
+      <c r="F222" s="2"/>
+      <c r="G222" s="2"/>
+      <c r="H222" s="2"/>
+      <c r="I222" s="2"/>
+      <c r="J222" s="2"/>
+      <c r="K222" s="2"/>
+      <c r="L222" s="2"/>
+      <c r="M222" s="2"/>
+      <c r="N222" s="2"/>
+      <c r="O222" s="2"/>
+      <c r="P222" s="2"/>
+      <c r="Q222" s="2"/>
+      <c r="R222" s="2"/>
+      <c r="S222" s="2"/>
+      <c r="T222" s="2"/>
+    </row>
+    <row r="223" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A223" s="2" t="s">
+        <v>650</v>
+      </c>
+      <c r="B223" s="2" t="s">
+        <v>651</v>
+      </c>
+      <c r="C223" s="2" t="s">
+        <v>652</v>
+      </c>
+      <c r="D223" s="2"/>
+      <c r="E223" s="2"/>
+      <c r="F223" s="2"/>
+      <c r="G223" s="2"/>
+      <c r="H223" s="2"/>
+      <c r="I223" s="2"/>
+      <c r="J223" s="2"/>
+      <c r="K223" s="2"/>
+      <c r="L223" s="2"/>
+      <c r="M223" s="2"/>
+      <c r="N223" s="2"/>
+      <c r="O223" s="2"/>
+      <c r="P223" s="2"/>
+      <c r="Q223" s="2"/>
+      <c r="R223" s="2"/>
+      <c r="S223" s="2"/>
+      <c r="T223" s="2"/>
+    </row>
+    <row r="224" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A224" s="2" t="s">
+        <v>653</v>
+      </c>
+      <c r="B224" s="2" t="s">
+        <v>654</v>
+      </c>
+      <c r="C224" s="2" t="s">
+        <v>655</v>
+      </c>
+      <c r="D224" s="2"/>
+      <c r="E224" s="2"/>
+      <c r="F224" s="2"/>
+      <c r="G224" s="2"/>
+      <c r="H224" s="2"/>
+      <c r="I224" s="2"/>
+      <c r="J224" s="2"/>
+      <c r="K224" s="2"/>
+      <c r="L224" s="2"/>
+      <c r="M224" s="2"/>
+      <c r="N224" s="2"/>
+      <c r="O224" s="2"/>
+      <c r="P224" s="2"/>
+      <c r="Q224" s="2"/>
+      <c r="R224" s="2"/>
+      <c r="S224" s="2"/>
+      <c r="T224" s="2"/>
+    </row>
+    <row r="225" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A225" s="2" t="s">
+        <v>656</v>
+      </c>
+      <c r="B225" s="2" t="s">
+        <v>657</v>
+      </c>
+      <c r="C225" s="2" t="s">
+        <v>658</v>
+      </c>
+      <c r="D225" s="2"/>
+      <c r="E225" s="2"/>
+      <c r="F225" s="2"/>
+      <c r="G225" s="2"/>
+      <c r="H225" s="2"/>
+      <c r="I225" s="2"/>
+      <c r="J225" s="2"/>
+      <c r="K225" s="2"/>
+      <c r="L225" s="2"/>
+      <c r="M225" s="2"/>
+      <c r="N225" s="2"/>
+      <c r="O225" s="2"/>
+      <c r="P225" s="2"/>
+      <c r="Q225" s="2"/>
+      <c r="R225" s="2"/>
+      <c r="S225" s="2"/>
+      <c r="T225" s="2"/>
+    </row>
+    <row r="226" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A226" s="2" t="s">
+        <v>659</v>
+      </c>
+      <c r="B226" s="2" t="s">
+        <v>660</v>
+      </c>
+      <c r="C226" s="2" t="s">
+        <v>661</v>
+      </c>
+      <c r="D226" s="2"/>
+      <c r="E226" s="2"/>
+      <c r="F226" s="2"/>
+      <c r="G226" s="2"/>
+      <c r="H226" s="2"/>
+      <c r="I226" s="2"/>
+      <c r="J226" s="2"/>
+      <c r="K226" s="2"/>
+      <c r="L226" s="2"/>
+      <c r="M226" s="2"/>
+      <c r="N226" s="2"/>
+      <c r="O226" s="2"/>
+      <c r="P226" s="2"/>
+      <c r="Q226" s="2"/>
+      <c r="R226" s="2"/>
+      <c r="S226" s="2"/>
+      <c r="T226" s="2"/>
+    </row>
+    <row r="227" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A227" s="2" t="s">
+        <v>662</v>
+      </c>
+      <c r="B227" s="2" t="s">
+        <v>663</v>
+      </c>
+      <c r="C227" s="2" t="s">
+        <v>664</v>
+      </c>
+      <c r="D227" s="2"/>
+      <c r="E227" s="2"/>
+      <c r="F227" s="2"/>
+      <c r="G227" s="2"/>
+      <c r="H227" s="2"/>
+      <c r="I227" s="2"/>
+      <c r="J227" s="2"/>
+      <c r="K227" s="2"/>
+      <c r="L227" s="2"/>
+      <c r="M227" s="2"/>
+      <c r="N227" s="2"/>
+      <c r="O227" s="2"/>
+      <c r="P227" s="2"/>
+      <c r="Q227" s="2"/>
+      <c r="R227" s="2"/>
+      <c r="S227" s="2"/>
+      <c r="T227" s="2"/>
+    </row>
+    <row r="228" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A228" s="2" t="s">
+        <v>665</v>
+      </c>
+      <c r="B228" s="2" t="s">
+        <v>666</v>
+      </c>
+      <c r="C228" s="2" t="s">
+        <v>667</v>
+      </c>
+      <c r="D228" s="2"/>
+      <c r="E228" s="2"/>
+      <c r="F228" s="2"/>
+      <c r="G228" s="2"/>
+      <c r="H228" s="2"/>
+      <c r="I228" s="2"/>
+      <c r="J228" s="2"/>
+      <c r="K228" s="2"/>
+      <c r="L228" s="2"/>
+      <c r="M228" s="2"/>
+      <c r="N228" s="2"/>
+      <c r="O228" s="2"/>
+      <c r="P228" s="2"/>
+      <c r="Q228" s="2"/>
+      <c r="R228" s="2"/>
+      <c r="S228" s="2"/>
+      <c r="T228" s="2"/>
+    </row>
+    <row r="229" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A229" s="2" t="s">
+        <v>668</v>
+      </c>
+      <c r="B229" s="2" t="s">
+        <v>669</v>
+      </c>
+      <c r="C229" s="2" t="s">
+        <v>670</v>
+      </c>
+      <c r="D229" s="2"/>
+      <c r="E229" s="2"/>
+      <c r="F229" s="2"/>
+      <c r="G229" s="2"/>
+      <c r="H229" s="2"/>
+      <c r="I229" s="2"/>
+      <c r="J229" s="2"/>
+      <c r="K229" s="2"/>
+      <c r="L229" s="2"/>
+      <c r="M229" s="2"/>
+      <c r="N229" s="2"/>
+      <c r="O229" s="2"/>
+      <c r="P229" s="2"/>
+      <c r="Q229" s="2"/>
+      <c r="R229" s="2"/>
+      <c r="S229" s="2"/>
+      <c r="T229" s="2"/>
+    </row>
+    <row r="230" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A230" s="2" t="s">
+        <v>671</v>
+      </c>
+      <c r="B230" s="2" t="s">
+        <v>672</v>
+      </c>
+      <c r="C230" s="2" t="s">
+        <v>673</v>
+      </c>
+      <c r="D230" s="2"/>
+      <c r="E230" s="2"/>
+      <c r="F230" s="2"/>
+      <c r="G230" s="2"/>
+      <c r="H230" s="2"/>
+      <c r="I230" s="2"/>
+      <c r="J230" s="2"/>
+      <c r="K230" s="2"/>
+      <c r="L230" s="2"/>
+      <c r="M230" s="2"/>
+      <c r="N230" s="2"/>
+      <c r="O230" s="2"/>
+      <c r="P230" s="2"/>
+      <c r="Q230" s="2"/>
+      <c r="R230" s="2"/>
+      <c r="S230" s="2"/>
+      <c r="T230" s="2"/>
+    </row>
+    <row r="231" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A231" s="2" t="s">
+        <v>674</v>
+      </c>
+      <c r="B231" s="2" t="s">
+        <v>675</v>
+      </c>
+      <c r="C231" s="2" t="s">
+        <v>676</v>
+      </c>
+      <c r="D231" s="2"/>
+      <c r="E231" s="2"/>
+      <c r="F231" s="2"/>
+      <c r="G231" s="2"/>
+      <c r="H231" s="2"/>
+      <c r="I231" s="2"/>
+      <c r="J231" s="2"/>
+      <c r="K231" s="2"/>
+      <c r="L231" s="2"/>
+      <c r="M231" s="2"/>
+      <c r="N231" s="2"/>
+      <c r="O231" s="2"/>
+      <c r="P231" s="2"/>
+      <c r="Q231" s="2"/>
+      <c r="R231" s="2"/>
+      <c r="S231" s="2"/>
+      <c r="T231" s="2"/>
+    </row>
+    <row r="232" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A232" s="2" t="s">
+        <v>677</v>
+      </c>
+      <c r="B232" s="2" t="s">
+        <v>678</v>
+      </c>
+      <c r="C232" s="2" t="s">
+        <v>679</v>
+      </c>
+      <c r="D232" s="2"/>
+      <c r="E232" s="2"/>
+      <c r="F232" s="2"/>
+      <c r="G232" s="2"/>
+      <c r="H232" s="2"/>
+      <c r="I232" s="2"/>
+      <c r="J232" s="2"/>
+      <c r="K232" s="2"/>
+      <c r="L232" s="2"/>
+      <c r="M232" s="2"/>
+      <c r="N232" s="2"/>
+      <c r="O232" s="2"/>
+      <c r="P232" s="2"/>
+      <c r="Q232" s="2"/>
+      <c r="R232" s="2"/>
+      <c r="S232" s="2"/>
+      <c r="T232" s="2"/>
+    </row>
+    <row r="233" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A233" s="2" t="s">
+        <v>680</v>
+      </c>
+      <c r="B233" s="2" t="s">
+        <v>681</v>
+      </c>
+      <c r="C233" s="2" t="s">
+        <v>682</v>
+      </c>
+      <c r="D233" s="2"/>
+      <c r="E233" s="2"/>
+      <c r="F233" s="2"/>
+      <c r="G233" s="2"/>
+      <c r="H233" s="2"/>
+      <c r="I233" s="2"/>
+      <c r="J233" s="2"/>
+      <c r="K233" s="2"/>
+      <c r="L233" s="2"/>
+      <c r="M233" s="2"/>
+      <c r="N233" s="2"/>
+      <c r="O233" s="2"/>
+      <c r="P233" s="2"/>
+      <c r="Q233" s="2"/>
+      <c r="R233" s="2"/>
+      <c r="S233" s="2"/>
+      <c r="T233" s="2"/>
+    </row>
+    <row r="234" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A234" s="2" t="s">
+        <v>683</v>
+      </c>
+      <c r="B234" s="2" t="s">
+        <v>684</v>
+      </c>
+      <c r="C234" s="2" t="s">
+        <v>685</v>
+      </c>
+      <c r="D234" s="2"/>
+      <c r="E234" s="2"/>
+      <c r="F234" s="2"/>
+      <c r="G234" s="2"/>
+      <c r="H234" s="2"/>
+      <c r="I234" s="2"/>
+      <c r="J234" s="2"/>
+      <c r="K234" s="2"/>
+      <c r="L234" s="2"/>
+      <c r="M234" s="2"/>
+      <c r="N234" s="2"/>
+      <c r="O234" s="2"/>
+      <c r="P234" s="2"/>
+      <c r="Q234" s="2"/>
+      <c r="R234" s="2"/>
+      <c r="S234" s="2"/>
+      <c r="T234" s="2"/>
+    </row>
+    <row r="235" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A235" s="2" t="s">
+        <v>686</v>
+      </c>
+      <c r="B235" s="2" t="s">
+        <v>687</v>
+      </c>
+      <c r="C235" s="2" t="s">
+        <v>688</v>
+      </c>
+      <c r="D235" s="2"/>
+      <c r="E235" s="2"/>
+      <c r="F235" s="2"/>
+      <c r="G235" s="2"/>
+      <c r="H235" s="2"/>
+      <c r="I235" s="2"/>
+      <c r="J235" s="2"/>
+      <c r="K235" s="2"/>
+      <c r="L235" s="2"/>
+      <c r="M235" s="2"/>
+      <c r="N235" s="2"/>
+      <c r="O235" s="2"/>
+      <c r="P235" s="2"/>
+      <c r="Q235" s="2"/>
+      <c r="R235" s="2"/>
+      <c r="S235" s="2"/>
+      <c r="T235" s="2"/>
+    </row>
+    <row r="236" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A236" s="2" t="s">
+        <v>689</v>
+      </c>
+      <c r="B236" s="2" t="s">
+        <v>690</v>
+      </c>
+      <c r="C236" s="2" t="s">
+        <v>691</v>
+      </c>
+      <c r="D236" s="2"/>
+      <c r="E236" s="2"/>
+      <c r="F236" s="2"/>
+      <c r="G236" s="2"/>
+      <c r="H236" s="2"/>
+      <c r="I236" s="2"/>
+      <c r="J236" s="2"/>
+      <c r="K236" s="2"/>
+      <c r="L236" s="2"/>
+      <c r="M236" s="2"/>
+      <c r="N236" s="2"/>
+      <c r="O236" s="2"/>
+      <c r="P236" s="2"/>
+      <c r="Q236" s="2"/>
+      <c r="R236" s="2"/>
+      <c r="S236" s="2"/>
+      <c r="T236" s="2"/>
+    </row>
+    <row r="237" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A237" s="2" t="s">
+        <v>692</v>
+      </c>
+      <c r="B237" s="2" t="s">
+        <v>693</v>
+      </c>
+      <c r="C237" s="2" t="s">
+        <v>694</v>
+      </c>
+      <c r="D237" s="2"/>
+      <c r="E237" s="2"/>
+      <c r="F237" s="2"/>
+      <c r="G237" s="2"/>
+      <c r="H237" s="2"/>
+      <c r="I237" s="2"/>
+      <c r="J237" s="2"/>
+      <c r="K237" s="2"/>
+      <c r="L237" s="2"/>
+      <c r="M237" s="2"/>
+      <c r="N237" s="2"/>
+      <c r="O237" s="2"/>
+      <c r="P237" s="2"/>
+      <c r="Q237" s="2"/>
+      <c r="R237" s="2"/>
+      <c r="S237" s="2"/>
+      <c r="T237" s="2"/>
+    </row>
+    <row r="238" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A238" s="2" t="s">
+        <v>695</v>
+      </c>
+      <c r="B238" s="2" t="s">
+        <v>696</v>
+      </c>
+      <c r="C238" s="2" t="s">
+        <v>697</v>
+      </c>
+      <c r="D238" s="2"/>
+      <c r="E238" s="2"/>
+      <c r="F238" s="2"/>
+      <c r="G238" s="2"/>
+      <c r="H238" s="2"/>
+      <c r="I238" s="2"/>
+      <c r="J238" s="2"/>
+      <c r="K238" s="2"/>
+      <c r="L238" s="2"/>
+      <c r="M238" s="2"/>
+      <c r="N238" s="2"/>
+      <c r="O238" s="2"/>
+      <c r="P238" s="2"/>
+      <c r="Q238" s="2"/>
+      <c r="R238" s="2"/>
+      <c r="S238" s="2"/>
+      <c r="T238" s="2"/>
+    </row>
+    <row r="239" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A239" s="2" t="s">
+        <v>698</v>
+      </c>
+      <c r="B239" s="2" t="s">
+        <v>699</v>
+      </c>
+      <c r="C239" s="2" t="s">
+        <v>700</v>
+      </c>
+      <c r="D239" s="2"/>
+      <c r="E239" s="2"/>
+      <c r="F239" s="2"/>
+      <c r="G239" s="2"/>
+      <c r="H239" s="2"/>
+      <c r="I239" s="2"/>
+      <c r="J239" s="2"/>
+      <c r="K239" s="2"/>
+      <c r="L239" s="2"/>
+      <c r="M239" s="2"/>
+      <c r="N239" s="2"/>
+      <c r="O239" s="2"/>
+      <c r="P239" s="2"/>
+      <c r="Q239" s="2"/>
+      <c r="R239" s="2"/>
+      <c r="S239" s="2"/>
+      <c r="T239" s="2"/>
+    </row>
+    <row r="240" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A240" s="2" t="s">
+        <v>701</v>
+      </c>
+      <c r="B240" s="2" t="s">
+        <v>702</v>
+      </c>
+      <c r="C240" s="2" t="s">
+        <v>703</v>
+      </c>
+      <c r="D240" s="2"/>
+      <c r="E240" s="2"/>
+      <c r="F240" s="2"/>
+      <c r="G240" s="2"/>
+      <c r="H240" s="2"/>
+      <c r="I240" s="2"/>
+      <c r="J240" s="2"/>
+      <c r="K240" s="2"/>
+      <c r="L240" s="2"/>
+      <c r="M240" s="2"/>
+      <c r="N240" s="2"/>
+      <c r="O240" s="2"/>
+      <c r="P240" s="2"/>
+      <c r="Q240" s="2"/>
+      <c r="R240" s="2"/>
+      <c r="S240" s="2"/>
+      <c r="T240" s="2"/>
+    </row>
+    <row r="241" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A241" s="2" t="s">
+        <v>704</v>
+      </c>
+      <c r="B241" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="C241" s="2" t="s">
+        <v>706</v>
+      </c>
+      <c r="D241" s="2"/>
+      <c r="E241" s="2"/>
+      <c r="F241" s="2"/>
+      <c r="G241" s="2"/>
+      <c r="H241" s="2"/>
+      <c r="I241" s="2"/>
+      <c r="J241" s="2"/>
+      <c r="K241" s="2"/>
+      <c r="L241" s="2"/>
+      <c r="M241" s="2"/>
+      <c r="N241" s="2"/>
+      <c r="O241" s="2"/>
+      <c r="P241" s="2"/>
+      <c r="Q241" s="2"/>
+      <c r="R241" s="2"/>
+      <c r="S241" s="2"/>
+      <c r="T241" s="2"/>
+    </row>
+    <row r="242" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A242" s="2" t="s">
+        <v>707</v>
+      </c>
+      <c r="B242" s="2" t="s">
+        <v>708</v>
+      </c>
+      <c r="C242" s="2" t="s">
+        <v>709</v>
+      </c>
+      <c r="D242" s="2"/>
+      <c r="E242" s="2"/>
+      <c r="F242" s="2"/>
+      <c r="G242" s="2"/>
+      <c r="H242" s="2"/>
+      <c r="I242" s="2"/>
+      <c r="J242" s="2"/>
+      <c r="K242" s="2"/>
+      <c r="L242" s="2"/>
+      <c r="M242" s="2"/>
+      <c r="N242" s="2"/>
+      <c r="O242" s="2"/>
+      <c r="P242" s="2"/>
+      <c r="Q242" s="2"/>
+      <c r="R242" s="2"/>
+      <c r="S242" s="2"/>
+      <c r="T242" s="2"/>
+    </row>
+    <row r="243" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A243" s="2" t="s">
+        <v>710</v>
+      </c>
+      <c r="B243" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="C243" s="2" t="s">
+        <v>712</v>
+      </c>
+      <c r="D243" s="2"/>
+      <c r="E243" s="2"/>
+      <c r="F243" s="2"/>
+      <c r="G243" s="2"/>
+      <c r="H243" s="2"/>
+      <c r="I243" s="2"/>
+      <c r="J243" s="2"/>
+      <c r="K243" s="2"/>
+      <c r="L243" s="2"/>
+      <c r="M243" s="2"/>
+      <c r="N243" s="2"/>
+      <c r="O243" s="2"/>
+      <c r="P243" s="2"/>
+      <c r="Q243" s="2"/>
+      <c r="R243" s="2"/>
+      <c r="S243" s="2"/>
+      <c r="T243" s="2"/>
+    </row>
+    <row r="244" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A244" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="B244" s="2" t="s">
+        <v>714</v>
+      </c>
+      <c r="C244" s="2" t="s">
+        <v>715</v>
+      </c>
+      <c r="D244" s="2"/>
+      <c r="E244" s="2"/>
+      <c r="F244" s="2"/>
+      <c r="G244" s="2"/>
+      <c r="H244" s="2"/>
+      <c r="I244" s="2"/>
+      <c r="J244" s="2"/>
+      <c r="K244" s="2"/>
+      <c r="L244" s="2"/>
+      <c r="M244" s="2"/>
+      <c r="N244" s="2"/>
+      <c r="O244" s="2"/>
+      <c r="P244" s="2"/>
+      <c r="Q244" s="2"/>
+      <c r="R244" s="2"/>
+      <c r="S244" s="2"/>
+      <c r="T244" s="2"/>
+    </row>
+    <row r="245" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A245" s="2" t="s">
+        <v>716</v>
+      </c>
+      <c r="B245" s="2" t="s">
+        <v>717</v>
+      </c>
+      <c r="C245" s="2" t="s">
+        <v>718</v>
+      </c>
+      <c r="D245" s="2"/>
+      <c r="E245" s="2"/>
+      <c r="F245" s="2"/>
+      <c r="G245" s="2"/>
+      <c r="H245" s="2"/>
+      <c r="I245" s="2"/>
+      <c r="J245" s="2"/>
+      <c r="K245" s="2"/>
+      <c r="L245" s="2"/>
+      <c r="M245" s="2"/>
+      <c r="N245" s="2"/>
+      <c r="O245" s="2"/>
+      <c r="P245" s="2"/>
+      <c r="Q245" s="2"/>
+      <c r="R245" s="2"/>
+      <c r="S245" s="2"/>
+      <c r="T245" s="2"/>
+    </row>
+    <row r="246" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A246" s="6" t="s">
+        <v>719</v>
+      </c>
+      <c r="B246" s="6" t="s">
+        <v>720</v>
+      </c>
+      <c r="C246" s="6" t="s">
+        <v>721</v>
+      </c>
+      <c r="D246" s="2"/>
+      <c r="E246" s="2"/>
+      <c r="F246" s="2"/>
+      <c r="G246" s="2"/>
+      <c r="H246" s="2"/>
+      <c r="I246" s="2"/>
+      <c r="J246" s="2"/>
+      <c r="K246" s="2"/>
+      <c r="L246" s="2"/>
+      <c r="M246" s="2"/>
+      <c r="N246" s="2"/>
+      <c r="O246" s="2"/>
+      <c r="P246" s="2"/>
+      <c r="Q246" s="2"/>
+      <c r="R246" s="2"/>
+      <c r="S246" s="2"/>
+      <c r="T246" s="2"/>
+    </row>
+    <row r="247" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A247" s="6" t="s">
+        <v>722</v>
+      </c>
+      <c r="B247" s="6" t="s">
+        <v>723</v>
+      </c>
+      <c r="C247" s="6" t="s">
+        <v>724</v>
+      </c>
+      <c r="D247" s="2"/>
+      <c r="E247" s="2"/>
+      <c r="F247" s="2"/>
+      <c r="G247" s="2"/>
+      <c r="H247" s="2"/>
+      <c r="I247" s="2"/>
+      <c r="J247" s="2"/>
+      <c r="K247" s="2"/>
+      <c r="L247" s="2"/>
+      <c r="M247" s="2"/>
+      <c r="N247" s="2"/>
+      <c r="O247" s="2"/>
+      <c r="P247" s="2"/>
+      <c r="Q247" s="2"/>
+      <c r="R247" s="2"/>
+      <c r="S247" s="2"/>
+      <c r="T247" s="2"/>
+    </row>
+    <row r="248" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A248" s="6" t="s">
+        <v>725</v>
+      </c>
+      <c r="B248" s="6" t="s">
+        <v>726</v>
+      </c>
+      <c r="C248" s="6" t="s">
+        <v>727</v>
+      </c>
+      <c r="D248" s="2"/>
+      <c r="E248" s="2"/>
+      <c r="F248" s="2"/>
+      <c r="G248" s="2"/>
+      <c r="H248" s="2"/>
+      <c r="I248" s="2"/>
+      <c r="J248" s="2"/>
+      <c r="K248" s="2"/>
+      <c r="L248" s="2"/>
+      <c r="M248" s="2"/>
+      <c r="N248" s="2"/>
+      <c r="O248" s="2"/>
+      <c r="P248" s="2"/>
+      <c r="Q248" s="2"/>
+      <c r="R248" s="2"/>
+      <c r="S248" s="2"/>
+      <c r="T248" s="2"/>
+    </row>
+    <row r="249" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A249" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="B249" s="2" t="s">
+        <v>729</v>
+      </c>
+      <c r="C249" s="2" t="s">
+        <v>730</v>
+      </c>
+      <c r="D249" s="2"/>
+      <c r="E249" s="2"/>
+      <c r="F249" s="2"/>
+      <c r="G249" s="2"/>
+      <c r="H249" s="2"/>
+      <c r="I249" s="2"/>
+      <c r="J249" s="2"/>
+      <c r="K249" s="2"/>
+      <c r="L249" s="2"/>
+      <c r="M249" s="2"/>
+      <c r="N249" s="2"/>
+      <c r="O249" s="2"/>
+      <c r="P249" s="2"/>
+      <c r="Q249" s="2"/>
+      <c r="R249" s="2"/>
+      <c r="S249" s="2"/>
+      <c r="T249" s="2"/>
+    </row>
+    <row r="250" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A250" s="2" t="s">
+        <v>731</v>
+      </c>
+      <c r="B250" s="2" t="s">
+        <v>732</v>
+      </c>
+      <c r="C250" s="2" t="s">
+        <v>733</v>
+      </c>
+      <c r="D250" s="2"/>
+      <c r="E250" s="2"/>
+      <c r="F250" s="2"/>
+      <c r="G250" s="2"/>
+      <c r="H250" s="2"/>
+      <c r="I250" s="2"/>
+      <c r="J250" s="2"/>
+      <c r="K250" s="2"/>
+      <c r="L250" s="2"/>
+      <c r="M250" s="2"/>
+      <c r="N250" s="2"/>
+      <c r="O250" s="2"/>
+      <c r="P250" s="2"/>
+      <c r="Q250" s="2"/>
+      <c r="R250" s="2"/>
+      <c r="S250" s="2"/>
+      <c r="T250" s="2"/>
+    </row>
+    <row r="251" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A251" s="2" t="s">
+        <v>734</v>
+      </c>
+      <c r="B251" s="2" t="s">
+        <v>735</v>
+      </c>
+      <c r="C251" s="2" t="s">
+        <v>736</v>
+      </c>
+      <c r="D251" s="2"/>
+      <c r="E251" s="2"/>
+      <c r="F251" s="2"/>
+      <c r="G251" s="2"/>
+      <c r="H251" s="2"/>
+      <c r="I251" s="2"/>
+      <c r="J251" s="2"/>
+      <c r="K251" s="2"/>
+      <c r="L251" s="2"/>
+      <c r="M251" s="2"/>
+      <c r="N251" s="2"/>
+      <c r="O251" s="2"/>
+      <c r="P251" s="2"/>
+      <c r="Q251" s="2"/>
+      <c r="R251" s="2"/>
+      <c r="S251" s="2"/>
+      <c r="T251" s="2"/>
+    </row>
+    <row r="252" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A252" s="2" t="s">
+        <v>737</v>
+      </c>
+      <c r="B252" s="2" t="s">
+        <v>738</v>
+      </c>
+      <c r="C252" s="2" t="s">
+        <v>739</v>
+      </c>
+      <c r="D252" s="2"/>
+      <c r="E252" s="2"/>
+      <c r="F252" s="2"/>
+      <c r="G252" s="2"/>
+      <c r="H252" s="2"/>
+      <c r="I252" s="2"/>
+      <c r="J252" s="2"/>
+      <c r="K252" s="2"/>
+      <c r="L252" s="2"/>
+      <c r="M252" s="2"/>
+      <c r="N252" s="2"/>
+      <c r="O252" s="2"/>
+      <c r="P252" s="2"/>
+      <c r="Q252" s="2"/>
+      <c r="R252" s="2"/>
+      <c r="S252" s="2"/>
+      <c r="T252" s="2"/>
+    </row>
+    <row r="253" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A253" s="2" t="s">
+        <v>740</v>
+      </c>
+      <c r="B253" s="2" t="s">
+        <v>741</v>
+      </c>
+      <c r="C253" s="2" t="s">
+        <v>742</v>
+      </c>
+      <c r="D253" s="2"/>
+      <c r="E253" s="2"/>
+      <c r="F253" s="2"/>
+      <c r="G253" s="2"/>
+      <c r="H253" s="2"/>
+      <c r="I253" s="2"/>
+      <c r="J253" s="2"/>
+      <c r="K253" s="2"/>
+      <c r="L253" s="2"/>
+      <c r="M253" s="2"/>
+      <c r="N253" s="2"/>
+      <c r="O253" s="2"/>
+      <c r="P253" s="2"/>
+      <c r="Q253" s="2"/>
+      <c r="R253" s="2"/>
+      <c r="S253" s="2"/>
+      <c r="T253" s="2"/>
+    </row>
+    <row r="254" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A254" s="2" t="s">
+        <v>743</v>
+      </c>
+      <c r="B254" s="2" t="s">
+        <v>744</v>
+      </c>
+      <c r="C254" s="2" t="s">
+        <v>745</v>
+      </c>
+      <c r="D254" s="2"/>
+      <c r="E254" s="2"/>
+      <c r="F254" s="2"/>
+      <c r="G254" s="2"/>
+      <c r="H254" s="2"/>
+      <c r="I254" s="2"/>
+      <c r="J254" s="2"/>
+      <c r="K254" s="2"/>
+      <c r="L254" s="2"/>
+      <c r="M254" s="2"/>
+      <c r="N254" s="2"/>
+      <c r="O254" s="2"/>
+      <c r="P254" s="2"/>
+      <c r="Q254" s="2"/>
+      <c r="R254" s="2"/>
+      <c r="S254" s="2"/>
+      <c r="T254" s="2"/>
+    </row>
     <row r="255" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="256" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="257" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -8616,7 +10361,6 @@
     <row r="996" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="997" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="998" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="999" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>